<commit_message>
chore(JdT): remplissage du journal de travail
</commit_message>
<xml_diff>
--- a/T-P_App-MatiasDenis-JDT.xlsx
+++ b/T-P_App-MatiasDenis-JDT.xlsx
@@ -5,10 +5,10 @@
   <workbookPr updateLinks="never" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\05-repertoires-ict-ssd (2022)\Deuxième année\P_App\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\05-repertoires-ict-ssd (2022)\Deuxième année\P_App\P_App-Bruteforce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBE0B49-D09A-4940-80E0-5640CC77B93C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C313E35-00D3-4ADB-85CF-EA2B53000DAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="42">
   <si>
     <t>Module :</t>
   </si>
@@ -165,6 +165,39 @@
   </si>
   <si>
     <t>Il a été dur de choisir mais finalement c'est le projet Bruteforce qui a été choisi. Le cahier des charges a été lu et compris.</t>
+  </si>
+  <si>
+    <t>Rédaction ébauche rapport de projet</t>
+  </si>
+  <si>
+    <t>Renseignement sur le bruteforce et le pentesting pour l'authentification</t>
+  </si>
+  <si>
+    <t>Création d'un schéma du fonctionnement du projet.</t>
+  </si>
+  <si>
+    <t>Rédaction de la page de garde, des différentes parties demandées, de la table des matières.</t>
+  </si>
+  <si>
+    <t>Lecture de plein de pages wikipédia, d'articles sur le sujet trouvés en ligne. Visionnage d'une vidéo pour comprendre les grands principes du pentesting.</t>
+  </si>
+  <si>
+    <t>Création d'un schéma du fonctionnement du programme.</t>
+  </si>
+  <si>
+    <t>Création d'un schéma représentant la logique du programme sur draw.io. A améliorer.</t>
+  </si>
+  <si>
+    <t>https://app.diagrams.net/</t>
+  </si>
+  <si>
+    <t>https://www.fortinet.com/fr/resources/cyberglossary/brute-force-attack
+https://fr.wikipedia.org/wiki/Test_d%27intrusion
+https://fr.wikipedia.org/wiki/Hacking_%C3%A9thique
+https://fr.wikipedia.org/wiki/Breach_and_attack_simulation
+https://www.youtube.com/watch?v=ZCuStkgjwM8
+https://www.youtube.com/watch?v=Mu1jlNSKytU
+https://chatgpt.com/share/691b1fbb-2888-8009-9e51-fc7f83414277</t>
   </si>
 </sst>
 </file>
@@ -1743,7 +1776,7 @@
   <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1999,7 +2032,9 @@
       <c r="B22" s="79">
         <v>2</v>
       </c>
-      <c r="C22" s="70"/>
+      <c r="C22" s="70" t="s">
+        <v>33</v>
+      </c>
       <c r="D22" s="59"/>
       <c r="E22" s="59"/>
       <c r="F22" s="59"/>
@@ -2010,7 +2045,9 @@
       <c r="B23" s="81">
         <v>3</v>
       </c>
-      <c r="C23" s="70"/>
+      <c r="C23" s="70" t="s">
+        <v>34</v>
+      </c>
       <c r="D23" s="59"/>
       <c r="E23" s="59"/>
       <c r="F23" s="59"/>
@@ -2021,7 +2058,9 @@
       <c r="B24" s="79">
         <v>4</v>
       </c>
-      <c r="C24" s="70"/>
+      <c r="C24" s="70" t="s">
+        <v>38</v>
+      </c>
       <c r="D24" s="59"/>
       <c r="E24" s="59"/>
       <c r="F24" s="59"/>
@@ -2357,27 +2396,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2407,27 +2446,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -3137,7 +3176,7 @@
   <dimension ref="A1:H153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -3190,23 +3229,45 @@
       </c>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="89"/>
+    <row r="4" spans="1:4" s="52" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="89" t="s">
+        <v>36</v>
+      </c>
       <c r="D4" s="10"/>
     </row>
-    <row r="5" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="89"/>
-      <c r="D5" s="93"/>
-    </row>
-    <row r="6" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="89"/>
-      <c r="D6" s="10"/>
+    <row r="5" spans="1:4" s="52" customFormat="1" ht="127.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="2">
+        <v>5</v>
+      </c>
+      <c r="C5" s="89" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="93" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="52" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="89" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="7" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
@@ -3280,7 +3341,7 @@
       </c>
       <c r="B18" s="47">
         <f>SUM(B3:B17)</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C18" s="87" t="s">
         <v>28</v>
@@ -4361,17 +4422,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Belge" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="14" ma:contentTypeDescription="Yeni belge oluşturun." ma:contentTypeScope="" ma:versionID="ee0afad02cec1cb5c008e069b7696935">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="071b3019c14a3acff1c11c5229ff0248" ns2:_="" ns3:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -4600,6 +4650,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
   <ds:schemaRefs>
@@ -4609,17 +4670,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15235525-7A96-4FDC-BE0C-FC0EC8076A2A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4636,4 +4686,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
doc(JdT, objectifs): mise à jour du journal de travail et des objectifs
</commit_message>
<xml_diff>
--- a/T-P_App-MatiasDenis-JDT.xlsx
+++ b/T-P_App-MatiasDenis-JDT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\05-repertoires-ict-ssd (2022)\Deuxième année\P_App\P_App-Bruteforce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61CA3BB0-0611-42AE-9340-63633034E4D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D7F745-B1BF-4770-8DB8-3A22D234081A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees" sheetId="7" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="54">
   <si>
     <t>Module :</t>
   </si>
@@ -198,6 +198,43 @@
 https://www.youtube.com/watch?v=ZCuStkgjwM8
 https://www.youtube.com/watch?v=Mu1jlNSKytU
 https://chatgpt.com/share/691b1fbb-2888-8009-9e51-fc7f83414277</t>
+  </si>
+  <si>
+    <t>Exemple code python</t>
+  </si>
+  <si>
+    <t>Exemple de code python trouvé dans une vidéo YouTube, il va être testé.</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/shorts/26giQUUh0Hs</t>
+  </si>
+  <si>
+    <t>Test code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nouveau code python </t>
+  </si>
+  <si>
+    <t>Le code python trouvé dans la vidéo youtube n'est pas du bruteforce car il retourne juste le temps qu'il met à trouver une combinaison de lettres qu'il fait. Il a été demandé à ChatGPT ce qu'il faisait et ce dernier a proposé une amélioration qui fait réellement du bruteforce avec une wordlist.txt</t>
+  </si>
+  <si>
+    <t>Le nouveau code lit donc le fichier wordlist.txt et renvoie une liste de mots de passe, le code s'arrête lorsque le mot de passe est trouvé et un message est affiché avec les données de l'utilisateur, le nombre de tentative et le temps écoulé. En moyenne il fait une tentative toutes les 0.00014 secondes. En partant du principe que l'affichage des messages prend du temps, on pourrait en gagner en les retirant. En effet après avoir enlever l'affichage des messages, on passe de une tentative chaque 0.00014 secondes à une tentative toutes les 0.000000048143 secondes.</t>
+  </si>
+  <si>
+    <t>Détermination des nouveaux objectifs du projet avec Mr. Melly</t>
+  </si>
+  <si>
+    <t>Après avoir été témoin de la vitesse du code, il a été décidé avec Mr. Melly de définir des objectifs plus précis: choisir une cible définie (db, site web, http, ftp, ssh) pour voir la différence de vitesse lorsque l'on rajoute les hash car on doit le calculer, le comparer, etc... 
+Mais également de voir si un mot de passe est trouvable rapidement avec un nombre de caractère élevé.</t>
+  </si>
+  <si>
+    <t>Recherche en ligne quant aux nouveaux objectifs</t>
+  </si>
+  <si>
+    <t>Jeudi 27.11</t>
+  </si>
+  <si>
+    <t>Tâche en cours, recherche de documentation en ligne pour les cibles: base de données, site web, etc…</t>
   </si>
 </sst>
 </file>
@@ -837,7 +874,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1124,6 +1161,12 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1776,7 +1819,7 @@
   <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2071,7 +2114,9 @@
       <c r="B25" s="79">
         <v>5</v>
       </c>
-      <c r="C25" s="70"/>
+      <c r="C25" s="70" t="s">
+        <v>42</v>
+      </c>
       <c r="D25" s="59"/>
       <c r="E25" s="59"/>
       <c r="F25" s="59"/>
@@ -2082,7 +2127,9 @@
       <c r="B26" s="81">
         <v>6</v>
       </c>
-      <c r="C26" s="70"/>
+      <c r="C26" s="70" t="s">
+        <v>45</v>
+      </c>
       <c r="D26" s="59"/>
       <c r="E26" s="59"/>
       <c r="F26" s="59"/>
@@ -2093,7 +2140,9 @@
       <c r="B27" s="79">
         <v>7</v>
       </c>
-      <c r="C27" s="70"/>
+      <c r="C27" s="70" t="s">
+        <v>46</v>
+      </c>
       <c r="D27" s="59"/>
       <c r="E27" s="59"/>
       <c r="F27" s="59"/>
@@ -2104,7 +2153,9 @@
       <c r="B28" s="79">
         <v>8</v>
       </c>
-      <c r="C28" s="71"/>
+      <c r="C28" s="71" t="s">
+        <v>49</v>
+      </c>
       <c r="D28" s="59"/>
       <c r="E28" s="59"/>
       <c r="F28" s="59"/>
@@ -2115,7 +2166,9 @@
       <c r="B29" s="81">
         <v>9</v>
       </c>
-      <c r="C29" s="71"/>
+      <c r="C29" s="71" t="s">
+        <v>51</v>
+      </c>
       <c r="D29" s="59"/>
       <c r="E29" s="59"/>
       <c r="F29" s="59"/>
@@ -2396,27 +2449,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2446,27 +2499,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -3173,10 +3226,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{080FAF2F-C534-499F-8C25-95E6F074E70C}">
   <sheetPr codeName="Feuil9"/>
-  <dimension ref="A1:H153"/>
+  <dimension ref="A1:H154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -3383,50 +3436,81 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="88"/>
-      <c r="D22" s="9"/>
+    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="100"/>
+      <c r="B22" s="101"/>
+      <c r="C22" s="100" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="100"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="89"/>
-      <c r="D23" s="10"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="10"/>
+      <c r="A23" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="4">
+        <v>1</v>
+      </c>
+      <c r="C23" s="88" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="54" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
+      <c r="C24" s="89" t="s">
+        <v>47</v>
+      </c>
       <c r="D24" s="10"/>
     </row>
-    <row r="25" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="10"/>
+    <row r="25" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="2">
+        <v>2</v>
+      </c>
+      <c r="C25" s="95" t="s">
+        <v>48</v>
+      </c>
       <c r="D25" s="10"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="33"/>
-    </row>
-    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="10"/>
+    </row>
+    <row r="26" spans="1:8" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="2">
+        <v>1</v>
+      </c>
+      <c r="C26" s="95" t="s">
+        <v>50</v>
+      </c>
       <c r="D26" s="10"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="30"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="10"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="33"/>
+    </row>
+    <row r="27" spans="1:8" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="2">
+        <v>1</v>
+      </c>
+      <c r="C27" s="95" t="s">
+        <v>53</v>
+      </c>
       <c r="D27" s="10"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
@@ -3456,7 +3540,7 @@
       <c r="H30" s="37"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
+      <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
@@ -3483,10 +3567,10 @@
       <c r="H33" s="37"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="50"/>
-      <c r="B34" s="50"/>
-      <c r="C34" s="51"/>
-      <c r="D34" s="51"/>
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
       <c r="F34" s="36"/>
       <c r="G34" s="37"/>
       <c r="H34" s="37"/>
@@ -3496,78 +3580,81 @@
       <c r="B35" s="50"/>
       <c r="C35" s="51"/>
       <c r="D35" s="51"/>
-      <c r="F35" s="38"/>
-      <c r="G35" s="39"/>
-      <c r="H35" s="39"/>
-    </row>
-    <row r="36" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="F36" s="40"/>
-      <c r="G36" s="40"/>
-      <c r="H36" s="40"/>
-    </row>
-    <row r="37" spans="1:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="47" t="s">
+      <c r="F35" s="36"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="37"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="50"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="51"/>
+      <c r="D36" s="51"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="39"/>
+      <c r="H36" s="39"/>
+    </row>
+    <row r="37" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="F37" s="40"/>
+      <c r="G37" s="40"/>
+      <c r="H37" s="40"/>
+    </row>
+    <row r="38" spans="1:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B37" s="47">
-        <f>SUM(B22:B36)</f>
-        <v>0</v>
-      </c>
-      <c r="C37" s="87" t="s">
+      <c r="B38" s="47">
+        <f>SUM(B23:B37)</f>
+        <v>6</v>
+      </c>
+      <c r="C38" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="D37" s="48"/>
-    </row>
-    <row r="38" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="49"/>
-      <c r="B38" s="49"/>
-      <c r="C38" s="49"/>
-      <c r="D38" s="49"/>
-    </row>
-    <row r="39" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="42" t="s">
+      <c r="D38" s="48"/>
+    </row>
+    <row r="39" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="49"/>
+      <c r="B39" s="49"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="49"/>
+    </row>
+    <row r="40" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B39" s="43">
+      <c r="B40" s="43">
         <v>3</v>
       </c>
-      <c r="C39" s="44" t="s">
+      <c r="C40" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="D39" s="53">
+      <c r="D40" s="53">
         <f>$D$20+7</f>
         <v>45978</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="45" t="s">
+    <row r="41" spans="1:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B40" s="46" t="s">
+      <c r="B41" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C40" s="45" t="s">
+      <c r="C41" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D40" s="45" t="s">
+      <c r="D41" s="45" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="88"/>
-      <c r="D41" s="9"/>
-    </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
+      <c r="A42" s="5"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="88"/>
+      <c r="D42" s="9"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
@@ -3612,7 +3699,7 @@
       <c r="D49" s="10"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="2"/>
+      <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="C50" s="10"/>
       <c r="D50" s="10"/>
@@ -3630,10 +3717,10 @@
       <c r="D52" s="10"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="50"/>
-      <c r="B53" s="50"/>
-      <c r="C53" s="51"/>
-      <c r="D53" s="51"/>
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="50"/>
@@ -3641,71 +3728,71 @@
       <c r="C54" s="51"/>
       <c r="D54" s="51"/>
     </row>
-    <row r="55" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="3"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="50"/>
+      <c r="B55" s="50"/>
+      <c r="C55" s="51"/>
+      <c r="D55" s="51"/>
     </row>
     <row r="56" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="47" t="s">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
+    </row>
+    <row r="57" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B56" s="47">
-        <f>SUM(B41:B55)</f>
+      <c r="B57" s="47">
+        <f>SUM(B42:B56)</f>
         <v>0</v>
       </c>
-      <c r="C56" s="87" t="s">
+      <c r="C57" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="D56" s="48"/>
-    </row>
-    <row r="57" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="49"/>
-      <c r="B57" s="49"/>
-      <c r="C57" s="49"/>
-      <c r="D57" s="49"/>
-    </row>
-    <row r="58" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="42" t="s">
+      <c r="D57" s="48"/>
+    </row>
+    <row r="58" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="49"/>
+      <c r="B58" s="49"/>
+      <c r="C58" s="49"/>
+      <c r="D58" s="49"/>
+    </row>
+    <row r="59" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B58" s="43">
+      <c r="B59" s="43">
         <v>4</v>
       </c>
-      <c r="C58" s="44" t="s">
+      <c r="C59" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="D58" s="53">
-        <f>$D$39+7</f>
+      <c r="D59" s="53">
+        <f>$D$40+7</f>
         <v>45985</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="45" t="s">
+    <row r="60" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B59" s="46" t="s">
+      <c r="B60" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C59" s="45" t="s">
+      <c r="C60" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D59" s="45" t="s">
+      <c r="D60" s="45" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="5"/>
-      <c r="B60" s="4"/>
-      <c r="C60" s="88"/>
-      <c r="D60" s="90"/>
-    </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-      <c r="B61" s="2"/>
-      <c r="C61" s="10"/>
-      <c r="D61" s="10"/>
+      <c r="A61" s="5"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="88"/>
+      <c r="D61" s="90"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
@@ -3750,7 +3837,7 @@
       <c r="D68" s="10"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="2"/>
+      <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="C69" s="10"/>
       <c r="D69" s="10"/>
@@ -3768,10 +3855,10 @@
       <c r="D71" s="10"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="50"/>
-      <c r="B72" s="50"/>
-      <c r="C72" s="51"/>
-      <c r="D72" s="51"/>
+      <c r="A72" s="2"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="10"/>
+      <c r="D72" s="10"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="50"/>
@@ -3779,71 +3866,71 @@
       <c r="C73" s="51"/>
       <c r="D73" s="51"/>
     </row>
-    <row r="74" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="3"/>
-      <c r="B74" s="3"/>
-      <c r="C74" s="11"/>
-      <c r="D74" s="11"/>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="50"/>
+      <c r="B74" s="50"/>
+      <c r="C74" s="51"/>
+      <c r="D74" s="51"/>
     </row>
     <row r="75" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="47" t="s">
+      <c r="A75" s="3"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="11"/>
+      <c r="D75" s="11"/>
+    </row>
+    <row r="76" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B75" s="47">
-        <f>SUM(B60:B74)</f>
+      <c r="B76" s="47">
+        <f>SUM(B61:B75)</f>
         <v>0</v>
       </c>
-      <c r="C75" s="87" t="s">
+      <c r="C76" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="D75" s="48"/>
-    </row>
-    <row r="76" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="49"/>
-      <c r="B76" s="49"/>
-      <c r="C76" s="49"/>
-      <c r="D76" s="49"/>
-    </row>
-    <row r="77" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="42" t="s">
+      <c r="D76" s="48"/>
+    </row>
+    <row r="77" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="49"/>
+      <c r="B77" s="49"/>
+      <c r="C77" s="49"/>
+      <c r="D77" s="49"/>
+    </row>
+    <row r="78" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B77" s="43">
+      <c r="B78" s="43">
         <v>5</v>
       </c>
-      <c r="C77" s="44" t="s">
+      <c r="C78" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="D77" s="53">
-        <f>$D$58+7</f>
+      <c r="D78" s="53">
+        <f>$D$59+7</f>
         <v>45992</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="45" t="s">
+    <row r="79" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B78" s="46" t="s">
+      <c r="B79" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C78" s="45" t="s">
+      <c r="C79" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D78" s="45" t="s">
+      <c r="D79" s="45" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="5"/>
-      <c r="B79" s="4"/>
-      <c r="C79" s="88"/>
-      <c r="D79" s="9"/>
-    </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="1"/>
-      <c r="B80" s="2"/>
-      <c r="C80" s="10"/>
-      <c r="D80" s="10"/>
+      <c r="A80" s="5"/>
+      <c r="B80" s="4"/>
+      <c r="C80" s="88"/>
+      <c r="D80" s="9"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
@@ -3888,7 +3975,7 @@
       <c r="D87" s="10"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="2"/>
+      <c r="A88" s="1"/>
       <c r="B88" s="2"/>
       <c r="C88" s="10"/>
       <c r="D88" s="10"/>
@@ -3906,10 +3993,10 @@
       <c r="D90" s="10"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="50"/>
-      <c r="B91" s="50"/>
-      <c r="C91" s="51"/>
-      <c r="D91" s="51"/>
+      <c r="A91" s="2"/>
+      <c r="B91" s="2"/>
+      <c r="C91" s="10"/>
+      <c r="D91" s="10"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="50"/>
@@ -3917,77 +4004,77 @@
       <c r="C92" s="51"/>
       <c r="D92" s="51"/>
     </row>
-    <row r="93" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="3"/>
-      <c r="B93" s="3"/>
-      <c r="C93" s="11"/>
-      <c r="D93" s="11"/>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="50"/>
+      <c r="B93" s="50"/>
+      <c r="C93" s="51"/>
+      <c r="D93" s="51"/>
     </row>
     <row r="94" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="47" t="s">
+      <c r="A94" s="3"/>
+      <c r="B94" s="3"/>
+      <c r="C94" s="11"/>
+      <c r="D94" s="11"/>
+    </row>
+    <row r="95" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B94" s="47">
-        <f>SUM(B79:B93)</f>
+      <c r="B95" s="47">
+        <f>SUM(B80:B94)</f>
         <v>0</v>
       </c>
-      <c r="C94" s="87" t="s">
+      <c r="C95" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="D94" s="48"/>
-    </row>
-    <row r="95" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="49"/>
-      <c r="B95" s="49"/>
-      <c r="C95" s="49"/>
-      <c r="D95" s="49"/>
-    </row>
-    <row r="96" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="42" t="s">
+      <c r="D95" s="48"/>
+    </row>
+    <row r="96" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A96" s="49"/>
+      <c r="B96" s="49"/>
+      <c r="C96" s="49"/>
+      <c r="D96" s="49"/>
+    </row>
+    <row r="97" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B96" s="43">
+      <c r="B97" s="43">
         <v>6</v>
       </c>
-      <c r="C96" s="44" t="s">
+      <c r="C97" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="D96" s="53">
-        <f>$D$77+7</f>
+      <c r="D97" s="53">
+        <f>$D$78+7</f>
         <v>45999</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="45" t="s">
+    <row r="98" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B97" s="46" t="s">
+      <c r="B98" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C97" s="45" t="s">
+      <c r="C98" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D97" s="45" t="s">
+      <c r="D98" s="45" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="5"/>
-      <c r="B98" s="4"/>
-      <c r="C98" s="88"/>
-      <c r="D98" s="91"/>
-    </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="1"/>
-      <c r="B99" s="2"/>
-      <c r="C99" s="89"/>
-      <c r="D99" s="93"/>
+      <c r="A99" s="5"/>
+      <c r="B99" s="4"/>
+      <c r="C99" s="88"/>
+      <c r="D99" s="91"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
-      <c r="C100" s="10"/>
-      <c r="D100" s="10"/>
+      <c r="C100" s="89"/>
+      <c r="D100" s="93"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
@@ -4026,7 +4113,7 @@
       <c r="D106" s="10"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="2"/>
+      <c r="A107" s="1"/>
       <c r="B107" s="2"/>
       <c r="C107" s="10"/>
       <c r="D107" s="10"/>
@@ -4044,10 +4131,10 @@
       <c r="D109" s="10"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="50"/>
-      <c r="B110" s="50"/>
-      <c r="C110" s="51"/>
-      <c r="D110" s="51"/>
+      <c r="A110" s="2"/>
+      <c r="B110" s="2"/>
+      <c r="C110" s="10"/>
+      <c r="D110" s="10"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="50"/>
@@ -4055,83 +4142,83 @@
       <c r="C111" s="51"/>
       <c r="D111" s="51"/>
     </row>
-    <row r="112" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="3"/>
-      <c r="B112" s="3"/>
-      <c r="C112" s="11"/>
-      <c r="D112" s="11"/>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="50"/>
+      <c r="B112" s="50"/>
+      <c r="C112" s="51"/>
+      <c r="D112" s="51"/>
     </row>
     <row r="113" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="47" t="s">
+      <c r="A113" s="3"/>
+      <c r="B113" s="3"/>
+      <c r="C113" s="11"/>
+      <c r="D113" s="11"/>
+    </row>
+    <row r="114" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B113" s="47">
-        <f>SUM(B98:B112)</f>
+      <c r="B114" s="47">
+        <f>SUM(B99:B113)</f>
         <v>0</v>
       </c>
-      <c r="C113" s="87" t="s">
+      <c r="C114" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="D113" s="48"/>
-    </row>
-    <row r="114" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A114" s="49"/>
-      <c r="B114" s="49"/>
-      <c r="C114" s="49"/>
-      <c r="D114" s="49"/>
-    </row>
-    <row r="115" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="42" t="s">
+      <c r="D114" s="48"/>
+    </row>
+    <row r="115" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A115" s="49"/>
+      <c r="B115" s="49"/>
+      <c r="C115" s="49"/>
+      <c r="D115" s="49"/>
+    </row>
+    <row r="116" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B115" s="43">
+      <c r="B116" s="43">
         <v>7</v>
       </c>
-      <c r="C115" s="44" t="s">
+      <c r="C116" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="D115" s="53">
-        <f>$D$96+7</f>
+      <c r="D116" s="53">
+        <f>$D$97+7</f>
         <v>46006</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="45" t="s">
+    <row r="117" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B116" s="46" t="s">
+      <c r="B117" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C116" s="45" t="s">
+      <c r="C117" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D116" s="45" t="s">
+      <c r="D117" s="45" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="5"/>
-      <c r="B117" s="4"/>
-      <c r="C117" s="88"/>
-      <c r="D117" s="9"/>
-    </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="1"/>
-      <c r="B118" s="2"/>
-      <c r="C118" s="92"/>
-      <c r="D118" s="10"/>
+      <c r="A118" s="5"/>
+      <c r="B118" s="4"/>
+      <c r="C118" s="88"/>
+      <c r="D118" s="9"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="2"/>
-      <c r="C119" s="89"/>
-      <c r="D119" s="93"/>
+      <c r="C119" s="92"/>
+      <c r="D119" s="10"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="2"/>
-      <c r="C120" s="10"/>
-      <c r="D120" s="10"/>
+      <c r="C120" s="89"/>
+      <c r="D120" s="93"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
@@ -4164,7 +4251,7 @@
       <c r="D125" s="10"/>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="2"/>
+      <c r="A126" s="1"/>
       <c r="B126" s="2"/>
       <c r="C126" s="10"/>
       <c r="D126" s="10"/>
@@ -4182,10 +4269,10 @@
       <c r="D128" s="10"/>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="50"/>
-      <c r="B129" s="50"/>
-      <c r="C129" s="51"/>
-      <c r="D129" s="51"/>
+      <c r="A129" s="2"/>
+      <c r="B129" s="2"/>
+      <c r="C129" s="10"/>
+      <c r="D129" s="10"/>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="50"/>
@@ -4193,76 +4280,76 @@
       <c r="C130" s="51"/>
       <c r="D130" s="51"/>
     </row>
-    <row r="131" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="3"/>
-      <c r="B131" s="3"/>
-      <c r="C131" s="11"/>
-      <c r="D131" s="11"/>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="50"/>
+      <c r="B131" s="50"/>
+      <c r="C131" s="51"/>
+      <c r="D131" s="51"/>
     </row>
     <row r="132" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="47" t="s">
+      <c r="A132" s="3"/>
+      <c r="B132" s="3"/>
+      <c r="C132" s="11"/>
+      <c r="D132" s="11"/>
+    </row>
+    <row r="133" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B132" s="47">
-        <f>SUM(B117:B131)</f>
+      <c r="B133" s="47">
+        <f>SUM(B118:B132)</f>
         <v>0</v>
       </c>
-      <c r="C132" s="87" t="s">
+      <c r="C133" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="D132" s="48"/>
-    </row>
-    <row r="133" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A133" s="49"/>
-      <c r="B133" s="49"/>
-      <c r="C133" s="49"/>
-      <c r="D133" s="49"/>
-    </row>
-    <row r="134" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="42" t="s">
+      <c r="D133" s="48"/>
+    </row>
+    <row r="134" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A134" s="49"/>
+      <c r="B134" s="49"/>
+      <c r="C134" s="49"/>
+      <c r="D134" s="49"/>
+    </row>
+    <row r="135" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A135" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B134" s="43">
+      <c r="B135" s="43">
         <v>8</v>
       </c>
-      <c r="C134" s="44" t="s">
+      <c r="C135" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="D134" s="53">
-        <f>$D$115+21</f>
+      <c r="D135" s="53">
+        <f>$D$116+21</f>
         <v>46027</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="45" t="s">
+    <row r="136" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B135" s="46" t="s">
+      <c r="B136" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C135" s="45" t="s">
+      <c r="C136" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D135" s="45" t="s">
+      <c r="D136" s="45" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="5"/>
-      <c r="B136" s="4"/>
-      <c r="C136" s="94"/>
-      <c r="D136" s="9"/>
-    </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="1"/>
-      <c r="B137" s="2"/>
-      <c r="C137" s="95"/>
-      <c r="D137" s="10"/>
+      <c r="A137" s="5"/>
+      <c r="B137" s="4"/>
+      <c r="C137" s="94"/>
+      <c r="D137" s="9"/>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
       <c r="B138" s="2"/>
-      <c r="C138" s="10"/>
+      <c r="C138" s="95"/>
       <c r="D138" s="10"/>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -4302,7 +4389,7 @@
       <c r="D144" s="10"/>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="2"/>
+      <c r="A145" s="1"/>
       <c r="B145" s="2"/>
       <c r="C145" s="10"/>
       <c r="D145" s="10"/>
@@ -4320,10 +4407,10 @@
       <c r="D147" s="10"/>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="50"/>
-      <c r="B148" s="50"/>
-      <c r="C148" s="51"/>
-      <c r="D148" s="51"/>
+      <c r="A148" s="2"/>
+      <c r="B148" s="2"/>
+      <c r="C148" s="10"/>
+      <c r="D148" s="10"/>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="50"/>
@@ -4331,50 +4418,56 @@
       <c r="C149" s="51"/>
       <c r="D149" s="51"/>
     </row>
-    <row r="150" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A150" s="3"/>
-      <c r="B150" s="3"/>
-      <c r="C150" s="11"/>
-      <c r="D150" s="11"/>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" s="50"/>
+      <c r="B150" s="50"/>
+      <c r="C150" s="51"/>
+      <c r="D150" s="51"/>
     </row>
     <row r="151" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A151" s="47" t="s">
+      <c r="A151" s="3"/>
+      <c r="B151" s="3"/>
+      <c r="C151" s="11"/>
+      <c r="D151" s="11"/>
+    </row>
+    <row r="152" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A152" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B151" s="47">
-        <f>SUM(B136:B150)</f>
+      <c r="B152" s="47">
+        <f>SUM(B137:B151)</f>
         <v>0</v>
       </c>
-      <c r="C151" s="87" t="s">
+      <c r="C152" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="D151" s="48"/>
-    </row>
-    <row r="152" spans="1:4" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A152" s="49"/>
-      <c r="B152" s="49"/>
-      <c r="C152" s="49"/>
-      <c r="D152" s="49"/>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="86" t="s">
+      <c r="D152" s="48"/>
+    </row>
+    <row r="153" spans="1:4" ht="14.25" x14ac:dyDescent="0.3">
+      <c r="A153" s="49"/>
+      <c r="B153" s="49"/>
+      <c r="C153" s="49"/>
+      <c r="D153" s="49"/>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="86" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="F35" xr:uid="{44460710-E505-40B8-8485-BA41A2FB3DB5}">
+    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="F36" xr:uid="{44460710-E505-40B8-8485-BA41A2FB3DB5}">
       <formula1>0</formula1>
       <formula2>DureePeriode-1</formula2>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="F27:F34 B3:B17 B22:B36 B41:B55 B60:B74 B79:B93 B98:B112 B117:B131 B136:B150" xr:uid="{B23B642E-0B29-4ED8-A409-C50EB7CC17BF}">
+    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="F28:F35 B3:B17 B23:B37 B42:B56 B61:B75 B80:B94 B99:B113 B118:B132 B137:B151" xr:uid="{B23B642E-0B29-4ED8-A409-C50EB7CC17BF}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B18 B37 B56 B75 B94 B113 B132 B151" xr:uid="{C02FA86D-12F2-40ED-8F5D-F7684A1E2EDD}">
+    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B18 B38 B57 B76 B95 B114 B133 B152" xr:uid="{C02FA86D-12F2-40ED-8F5D-F7684A1E2EDD}">
       <formula1>0</formula1>
       <formula2>NbPerWeek * NbQuartPer</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A17 A22:A36 A41:A55 A60:A74 A79:A93 A98:A112 A117:A131 A136:A150" xr:uid="{BCBC0613-73E6-47AF-B0DB-7981EF783ABA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A17 A23:A37 A42:A56 A61:A75 A80:A94 A99:A113 A118:A132 A137:A151" xr:uid="{BCBC0613-73E6-47AF-B0DB-7981EF783ABA}">
       <formula1>lstTasks</formula1>
     </dataValidation>
   </dataValidations>
@@ -4422,17 +4515,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Belge" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="14" ma:contentTypeDescription="Yeni belge oluşturun." ma:contentTypeScope="" ma:versionID="ee0afad02cec1cb5c008e069b7696935">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="071b3019c14a3acff1c11c5229ff0248" ns2:_="" ns3:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -4661,6 +4743,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
   <ds:schemaRefs>
@@ -4670,17 +4763,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15235525-7A96-4FDC-BE0C-FC0EC8076A2A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4697,4 +4779,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
doc(JdT): mise à jour du journal de travail.
</commit_message>
<xml_diff>
--- a/T-P_App-MatiasDenis-JDT.xlsx
+++ b/T-P_App-MatiasDenis-JDT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\05-repertoires-ict-ssd (2022)\Deuxième année\P_App\P_App-Bruteforce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D7F745-B1BF-4770-8DB8-3A22D234081A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F1E536-0E83-44B4-A832-5B00DF2266D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="56">
   <si>
     <t>Module :</t>
   </si>
@@ -235,6 +235,12 @@
   </si>
   <si>
     <t>Tâche en cours, recherche de documentation en ligne pour les cibles: base de données, site web, etc…</t>
+  </si>
+  <si>
+    <t>Rédaction du rapport de projet</t>
+  </si>
+  <si>
+    <t>Rédaction du chapitre Explications du code avec beaucoup de détails sur les différentes parties du code.</t>
   </si>
 </sst>
 </file>
@@ -1151,6 +1157,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1161,12 +1173,6 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1819,7 +1825,7 @@
   <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2035,10 +2041,10 @@
     </row>
     <row r="19" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="78"/>
-      <c r="B19" s="96" t="s">
+      <c r="B19" s="98" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="97"/>
+      <c r="C19" s="99"/>
       <c r="D19" s="59"/>
       <c r="E19" s="59"/>
       <c r="F19" s="59"/>
@@ -2179,7 +2185,9 @@
       <c r="B30" s="79">
         <v>10</v>
       </c>
-      <c r="C30" s="70"/>
+      <c r="C30" s="70" t="s">
+        <v>54</v>
+      </c>
       <c r="D30" s="59"/>
       <c r="E30" s="59"/>
       <c r="F30" s="59"/>
@@ -2558,7 +2566,7 @@
     </row>
     <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="100" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="16">
@@ -2567,7 +2575,7 @@
     </row>
     <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
-      <c r="B4" s="99"/>
+      <c r="B4" s="101"/>
       <c r="C4" s="22">
         <v>0</v>
       </c>
@@ -3228,8 +3236,8 @@
   <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:H154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -3437,12 +3445,12 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="100"/>
-      <c r="B22" s="101"/>
-      <c r="C22" s="100" t="s">
+      <c r="A22" s="96"/>
+      <c r="B22" s="97"/>
+      <c r="C22" s="96" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="100"/>
+      <c r="D22" s="96"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
@@ -3502,7 +3510,7 @@
         <v>51</v>
       </c>
       <c r="B27" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C27" s="95" t="s">
         <v>53</v>
@@ -3512,10 +3520,16 @@
       <c r="G27" s="30"/>
       <c r="H27" s="30"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="10"/>
+    <row r="28" spans="1:8" ht="27" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="2">
+        <v>2</v>
+      </c>
+      <c r="C28" s="95" t="s">
+        <v>55</v>
+      </c>
       <c r="D28" s="10"/>
       <c r="F28" s="36"/>
       <c r="G28" s="37"/>
@@ -3608,7 +3622,7 @@
       </c>
       <c r="B38" s="47">
         <f>SUM(B23:B37)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C38" s="87" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
doc(JdT): rédaction du journal de travail
</commit_message>
<xml_diff>
--- a/T-P_App-MatiasDenis-JDT.xlsx
+++ b/T-P_App-MatiasDenis-JDT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\05-repertoires-ict-ssd (2022)\Deuxième année\P_App\P_App-Bruteforce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F1E536-0E83-44B4-A832-5B00DF2266D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5922C3B-E461-4AF5-A9B6-F4FC4A5E2ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="67">
   <si>
     <t>Module :</t>
   </si>
@@ -164,9 +164,6 @@
     <t>Choix du projet et prise de connaissance du CdC</t>
   </si>
   <si>
-    <t>Il a été dur de choisir mais finalement c'est le projet Bruteforce qui a été choisi. Le cahier des charges a été lu et compris.</t>
-  </si>
-  <si>
     <t>Rédaction ébauche rapport de projet</t>
   </si>
   <si>
@@ -174,12 +171,6 @@
   </si>
   <si>
     <t>Création d'un schéma du fonctionnement du projet.</t>
-  </si>
-  <si>
-    <t>Rédaction de la page de garde, des différentes parties demandées, de la table des matières.</t>
-  </si>
-  <si>
-    <t>Lecture de plein de pages wikipédia, d'articles sur le sujet trouvés en ligne. Visionnage d'une vidéo pour comprendre les grands principes du pentesting.</t>
   </si>
   <si>
     <t>Création d'un schéma du fonctionnement du programme.</t>
@@ -215,12 +206,6 @@
     <t xml:space="preserve">Nouveau code python </t>
   </si>
   <si>
-    <t>Le code python trouvé dans la vidéo youtube n'est pas du bruteforce car il retourne juste le temps qu'il met à trouver une combinaison de lettres qu'il fait. Il a été demandé à ChatGPT ce qu'il faisait et ce dernier a proposé une amélioration qui fait réellement du bruteforce avec une wordlist.txt</t>
-  </si>
-  <si>
-    <t>Le nouveau code lit donc le fichier wordlist.txt et renvoie une liste de mots de passe, le code s'arrête lorsque le mot de passe est trouvé et un message est affiché avec les données de l'utilisateur, le nombre de tentative et le temps écoulé. En moyenne il fait une tentative toutes les 0.00014 secondes. En partant du principe que l'affichage des messages prend du temps, on pourrait en gagner en les retirant. En effet après avoir enlever l'affichage des messages, on passe de une tentative chaque 0.00014 secondes à une tentative toutes les 0.000000048143 secondes.</t>
-  </si>
-  <si>
     <t>Détermination des nouveaux objectifs du projet avec Mr. Melly</t>
   </si>
   <si>
@@ -240,7 +225,55 @@
     <t>Rédaction du rapport de projet</t>
   </si>
   <si>
-    <t>Rédaction du chapitre Explications du code avec beaucoup de détails sur les différentes parties du code.</t>
+    <t>Adaptation du schéma</t>
+  </si>
+  <si>
+    <t>Après réflexion et conseils du professeur, le schéma doit être adapté car il n'est pas assez explicite. Tâche en cours.</t>
+  </si>
+  <si>
+    <t>Fin de la rédaction du chapitre Explications du code avec beaucoup de détails sur les différentes parties du code. Tâche terminée.</t>
+  </si>
+  <si>
+    <t>Rédaction du chapitre Explications du code avec beaucoup de détails sur les différentes parties du code. Tâche en cours.</t>
+  </si>
+  <si>
+    <t>Le nouveau code lit donc le fichier wordlist.txt et renvoie une liste de mots de passe, le code s'arrête lorsque le mot de passe est trouvé et un message est affiché avec les données de l'utilisateur, le nombre de tentative et le temps écoulé. En moyenne il fait une tentative toutes les 0.00014 secondes. En partant du principe que l'affichage des messages prend du temps, on pourrait en gagner en les retirant. En effet après avoir enlever l'affichage des messages, on passe de une tentative chaque 0.00014 secondes à une tentative toutes les 0.000000048143 secondes. Tâche terminée.</t>
+  </si>
+  <si>
+    <t>Le code python trouvé dans la vidéo youtube n'est pas du bruteforce car il retourne juste le temps qu'il met à trouver une combinaison de lettres qu'il fait. Il a été demandé à ChatGPT ce qu'il faisait et ce dernier a proposé une amélioration qui fait réellement du bruteforce avec une wordlist.txt. Tâche terminée.</t>
+  </si>
+  <si>
+    <t>Lecture de plein de pages wikipédia, d'articles sur le sujet trouvés en ligne. Visionnage d'une vidéo pour comprendre les grands principes du pentesting. Tâche terminée.</t>
+  </si>
+  <si>
+    <t>Rédaction de la page de garde, des différentes parties demandées, de la table des matières. Tâche terminée.</t>
+  </si>
+  <si>
+    <t>Il a été dur de choisir mais finalement c'est le projet Bruteforce qui a été choisi. Le cahier des charges a été lu et compris. Tâche terminée.</t>
+  </si>
+  <si>
+    <t>Mise en place d'un serveur FTP avec Docker</t>
+  </si>
+  <si>
+    <t>Connexion FTP depuis Python</t>
+  </si>
+  <si>
+    <t>Bruteforce FTP réel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tests </t>
+  </si>
+  <si>
+    <t>Installation de Docker et création du fichier docker-compose.yml, déploiement du serveur FTP local, vérification du serveur FTP via FileZilla, validation que le mot de pas réel fonctionne bien sur FTP. Tâche terminée.</t>
+  </si>
+  <si>
+    <t>Création du script test_ftp.py pour valider une connexion FTP Python -&gt; Docker, tests de connexion FTP (auth OK), intégration d'une fonction de test FTP dans le bruteforce (connexion réelle), sécurisation du script (blocage sur 127.0.0.1 uniquement). Tâche terminée.</t>
+  </si>
+  <si>
+    <t>Modification du script principal pour utiliser le test FTP réel, tests de bruteforce avec wordlist simple, validation de la détection correcte du mot de passe via FTP, mesure du temps et du nombre de tentatives. Tâche terminée.</t>
+  </si>
+  <si>
+    <t>Tests du programme avec des positions différentes du mot de passe dans la wordlist et calcul du temps. D'autres tests à faire afin d'optimiser le programme. Tâche en cours.</t>
   </si>
 </sst>
 </file>
@@ -1825,7 +1858,7 @@
   <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2082,7 +2115,7 @@
         <v>2</v>
       </c>
       <c r="C22" s="70" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D22" s="59"/>
       <c r="E22" s="59"/>
@@ -2095,7 +2128,7 @@
         <v>3</v>
       </c>
       <c r="C23" s="70" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D23" s="59"/>
       <c r="E23" s="59"/>
@@ -2108,7 +2141,7 @@
         <v>4</v>
       </c>
       <c r="C24" s="70" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D24" s="59"/>
       <c r="E24" s="59"/>
@@ -2121,7 +2154,7 @@
         <v>5</v>
       </c>
       <c r="C25" s="70" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D25" s="59"/>
       <c r="E25" s="59"/>
@@ -2134,7 +2167,7 @@
         <v>6</v>
       </c>
       <c r="C26" s="70" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D26" s="59"/>
       <c r="E26" s="59"/>
@@ -2147,7 +2180,7 @@
         <v>7</v>
       </c>
       <c r="C27" s="70" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D27" s="59"/>
       <c r="E27" s="59"/>
@@ -2160,7 +2193,7 @@
         <v>8</v>
       </c>
       <c r="C28" s="71" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D28" s="59"/>
       <c r="E28" s="59"/>
@@ -2173,7 +2206,7 @@
         <v>9</v>
       </c>
       <c r="C29" s="71" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D29" s="59"/>
       <c r="E29" s="59"/>
@@ -2186,7 +2219,7 @@
         <v>10</v>
       </c>
       <c r="C30" s="70" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D30" s="59"/>
       <c r="E30" s="59"/>
@@ -2198,7 +2231,9 @@
       <c r="B31" s="79">
         <v>11</v>
       </c>
-      <c r="C31" s="70"/>
+      <c r="C31" s="70" t="s">
+        <v>50</v>
+      </c>
       <c r="D31" s="59"/>
       <c r="E31" s="59"/>
       <c r="F31" s="59"/>
@@ -2209,7 +2244,9 @@
       <c r="B32" s="81">
         <v>12</v>
       </c>
-      <c r="C32" s="70"/>
+      <c r="C32" s="70" t="s">
+        <v>59</v>
+      </c>
       <c r="D32" s="59"/>
       <c r="E32" s="59"/>
       <c r="F32" s="59"/>
@@ -2220,7 +2257,9 @@
       <c r="B33" s="79">
         <v>13</v>
       </c>
-      <c r="C33" s="70"/>
+      <c r="C33" s="70" t="s">
+        <v>60</v>
+      </c>
       <c r="D33" s="59"/>
       <c r="E33" s="59"/>
       <c r="F33" s="59"/>
@@ -2231,7 +2270,9 @@
       <c r="B34" s="79">
         <v>14</v>
       </c>
-      <c r="C34" s="71"/>
+      <c r="C34" s="71" t="s">
+        <v>61</v>
+      </c>
       <c r="D34" s="59"/>
       <c r="E34" s="59"/>
       <c r="F34" s="59"/>
@@ -2242,7 +2283,9 @@
       <c r="B35" s="81">
         <v>15</v>
       </c>
-      <c r="C35" s="71"/>
+      <c r="C35" s="71" t="s">
+        <v>62</v>
+      </c>
       <c r="D35" s="59"/>
       <c r="E35" s="59"/>
       <c r="F35" s="59"/>
@@ -3236,8 +3279,8 @@
   <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:H154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -3286,48 +3329,48 @@
         <v>2</v>
       </c>
       <c r="C3" s="88" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="D3" s="9"/>
     </row>
     <row r="4" spans="1:4" s="52" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
       </c>
       <c r="C4" s="89" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="D4" s="10"/>
     </row>
     <row r="5" spans="1:4" s="52" customFormat="1" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="2">
         <v>5</v>
       </c>
       <c r="C5" s="89" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="D5" s="93" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="52" customFormat="1" ht="54" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
       </c>
       <c r="C6" s="89" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
@@ -3448,57 +3491,57 @@
       <c r="A22" s="96"/>
       <c r="B22" s="97"/>
       <c r="C22" s="96" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D22" s="96"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B23" s="4">
         <v>1</v>
       </c>
       <c r="C23" s="88" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="54" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B24" s="2">
         <v>1</v>
       </c>
       <c r="C24" s="89" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D24" s="10"/>
     </row>
     <row r="25" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B25" s="2">
         <v>2</v>
       </c>
       <c r="C25" s="95" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D25" s="10"/>
     </row>
     <row r="26" spans="1:8" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B26" s="2">
         <v>1</v>
       </c>
       <c r="C26" s="95" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D26" s="10"/>
       <c r="F26" s="31"/>
@@ -3507,13 +3550,13 @@
     </row>
     <row r="27" spans="1:8" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B27" s="2">
         <v>2</v>
       </c>
       <c r="C27" s="95" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D27" s="10"/>
       <c r="F27" s="34"/>
@@ -3522,13 +3565,13 @@
     </row>
     <row r="28" spans="1:8" ht="27" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B28" s="2">
         <v>2</v>
       </c>
       <c r="C28" s="95" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D28" s="10"/>
       <c r="F28" s="36"/>
@@ -3664,40 +3707,76 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="88"/>
+    <row r="42" spans="1:8" ht="27" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" s="4">
+        <v>2</v>
+      </c>
+      <c r="C42" s="95" t="s">
+        <v>52</v>
+      </c>
       <c r="D42" s="9"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="10"/>
+    <row r="43" spans="1:8" ht="27" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" s="2">
+        <v>1</v>
+      </c>
+      <c r="C43" s="95" t="s">
+        <v>51</v>
+      </c>
       <c r="D43" s="10"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="10"/>
+    <row r="44" spans="1:8" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B44" s="2">
+        <v>1</v>
+      </c>
+      <c r="C44" s="95" t="s">
+        <v>63</v>
+      </c>
       <c r="D44" s="10"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="10"/>
+    <row r="45" spans="1:8" ht="54" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B45" s="2">
+        <v>2</v>
+      </c>
+      <c r="C45" s="95" t="s">
+        <v>64</v>
+      </c>
       <c r="D45" s="10"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="10"/>
+    <row r="46" spans="1:8" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B46" s="2">
+        <v>2</v>
+      </c>
+      <c r="C46" s="95" t="s">
+        <v>65</v>
+      </c>
       <c r="D46" s="10"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="10"/>
+    <row r="47" spans="1:8" ht="27" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B47" s="2">
+        <v>1</v>
+      </c>
+      <c r="C47" s="95" t="s">
+        <v>66</v>
+      </c>
       <c r="D47" s="10"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -3760,7 +3839,7 @@
       </c>
       <c r="B57" s="47">
         <f>SUM(B42:B56)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C57" s="87" t="s">
         <v>28</v>
@@ -3803,13 +3882,17 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="5"/>
+      <c r="A61" s="5" t="s">
+        <v>62</v>
+      </c>
       <c r="B61" s="4"/>
       <c r="C61" s="88"/>
       <c r="D61" s="90"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
+    <row r="62" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="B62" s="2"/>
       <c r="C62" s="10"/>
       <c r="D62" s="10"/>

</xml_diff>

<commit_message>
doc(JdT): correction et rédaction du journal de travail
</commit_message>
<xml_diff>
--- a/T-P_App-MatiasDenis-JDT.xlsx
+++ b/T-P_App-MatiasDenis-JDT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\05-repertoires-ict-ssd (2022)\Deuxième année\P_App\P_App-Bruteforce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5922C3B-E461-4AF5-A9B6-F4FC4A5E2ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFEEA9C3-D9DD-495E-BCA1-D78D3595E508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees" sheetId="7" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <definedName name="objFooterDiagram">DiagramFooter!$B$3:$C$4</definedName>
     <definedName name="objPlanifWeek">PlanificationWeek!$A$1:$D$14</definedName>
     <definedName name="objRealizedWeek" localSheetId="4">achievementWeek!$A$1:$D$19</definedName>
-    <definedName name="objRealizedWeek" localSheetId="5">JNLTRAV!$A$1:$D$19</definedName>
+    <definedName name="objRealizedWeek" localSheetId="5">JNLTRAV!$A$1:$D$18</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Donnees!$A$1:$G$47</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="77">
   <si>
     <t>Module :</t>
   </si>
@@ -170,16 +170,10 @@
     <t>Renseignement sur le bruteforce et le pentesting pour l'authentification</t>
   </si>
   <si>
-    <t>Création d'un schéma du fonctionnement du projet.</t>
-  </si>
-  <si>
     <t>Création d'un schéma du fonctionnement du programme.</t>
   </si>
   <si>
     <t>Création d'un schéma représentant la logique du programme sur draw.io. A améliorer.</t>
-  </si>
-  <si>
-    <t>https://app.diagrams.net/</t>
   </si>
   <si>
     <t>https://www.fortinet.com/fr/resources/cyberglossary/brute-force-attack
@@ -219,9 +213,6 @@
     <t>Jeudi 27.11</t>
   </si>
   <si>
-    <t>Tâche en cours, recherche de documentation en ligne pour les cibles: base de données, site web, etc…</t>
-  </si>
-  <si>
     <t>Rédaction du rapport de projet</t>
   </si>
   <si>
@@ -234,24 +225,12 @@
     <t>Fin de la rédaction du chapitre Explications du code avec beaucoup de détails sur les différentes parties du code. Tâche terminée.</t>
   </si>
   <si>
-    <t>Rédaction du chapitre Explications du code avec beaucoup de détails sur les différentes parties du code. Tâche en cours.</t>
-  </si>
-  <si>
-    <t>Le nouveau code lit donc le fichier wordlist.txt et renvoie une liste de mots de passe, le code s'arrête lorsque le mot de passe est trouvé et un message est affiché avec les données de l'utilisateur, le nombre de tentative et le temps écoulé. En moyenne il fait une tentative toutes les 0.00014 secondes. En partant du principe que l'affichage des messages prend du temps, on pourrait en gagner en les retirant. En effet après avoir enlever l'affichage des messages, on passe de une tentative chaque 0.00014 secondes à une tentative toutes les 0.000000048143 secondes. Tâche terminée.</t>
-  </si>
-  <si>
     <t>Le code python trouvé dans la vidéo youtube n'est pas du bruteforce car il retourne juste le temps qu'il met à trouver une combinaison de lettres qu'il fait. Il a été demandé à ChatGPT ce qu'il faisait et ce dernier a proposé une amélioration qui fait réellement du bruteforce avec une wordlist.txt. Tâche terminée.</t>
   </si>
   <si>
-    <t>Lecture de plein de pages wikipédia, d'articles sur le sujet trouvés en ligne. Visionnage d'une vidéo pour comprendre les grands principes du pentesting. Tâche terminée.</t>
-  </si>
-  <si>
     <t>Rédaction de la page de garde, des différentes parties demandées, de la table des matières. Tâche terminée.</t>
   </si>
   <si>
-    <t>Il a été dur de choisir mais finalement c'est le projet Bruteforce qui a été choisi. Le cahier des charges a été lu et compris. Tâche terminée.</t>
-  </si>
-  <si>
     <t>Mise en place d'un serveur FTP avec Docker</t>
   </si>
   <si>
@@ -274,6 +253,57 @@
   </si>
   <si>
     <t>Tests du programme avec des positions différentes du mot de passe dans la wordlist et calcul du temps. D'autres tests à faire afin d'optimiser le programme. Tâche en cours.</t>
+  </si>
+  <si>
+    <t>Maladie.</t>
+  </si>
+  <si>
+    <t>Lecture de plein de pages wikipédia, d'articles sur le sujet trouvés en ligne. Visionnage d'une vidéo pour comprendre les grands principes du pentesting. Demande d'explications à l'IA. Tâche terminée.</t>
+  </si>
+  <si>
+    <t>Jeudi 20.11</t>
+  </si>
+  <si>
+    <t>Max. 18</t>
+  </si>
+  <si>
+    <t>Jeudi 06.11</t>
+  </si>
+  <si>
+    <t>Jeudi 13.11</t>
+  </si>
+  <si>
+    <t>Jeudi 11.12</t>
+  </si>
+  <si>
+    <t>Jeudi 04.12</t>
+  </si>
+  <si>
+    <t>Mise au propre du journal de travail</t>
+  </si>
+  <si>
+    <t>C'est le projet Bruteforce qui a été choisi. Le cahier des charges a été lu et compris. Tâche terminée.</t>
+  </si>
+  <si>
+    <t>Il y avait confusion dans les dates où le projet a été effectué mais tout est juste maintenant. Tâche terminée.</t>
+  </si>
+  <si>
+    <t>Changement dans le rapport de travail: réduction du nombre de page pour s'aligner avec ce qui est demandé dans le cahier des charges. Tâche en cours.</t>
+  </si>
+  <si>
+    <t>Tests</t>
+  </si>
+  <si>
+    <t>Le nouveau code, donné par ChatGPT, lit donc le fichier wordlist.txt et renvoie une liste de mots de passe, le code s'arrête lorsque le mot de passe est trouvé et un message est affiché avec les données de l'utilisateur, le nombre de tentative et le temps écoulé. En moyenne il fait une tentative toutes les 0.00014 secondes. En partant du principe que l'affichage des messages prend du temps, on pourrait en gagner en les retirant. En effet après avoir enlever l'affichage des messages, on passe de une tentative chaque 0.00014 secondes à une tentative toutes les 0.000000048143 secondes. Tâche terminée.</t>
+  </si>
+  <si>
+    <t>Recherche de documentation en ligne pour les cibles: base de données, site web, etc… Tâche terminée.</t>
+  </si>
+  <si>
+    <t>Rédaction du chapitre Explications du code avec beaucoup de détails sur les différentes parties du code. Tâche terminée.</t>
+  </si>
+  <si>
+    <t>Adaptation du schéma pour qu'il soit plus facile à comprendre lorsque l'on a pas encore vu le projet.</t>
   </si>
 </sst>
 </file>
@@ -474,7 +504,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="52">
     <border>
       <left/>
       <right/>
@@ -903,6 +933,226 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -913,7 +1163,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1167,13 +1417,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -1195,6 +1438,179 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="13" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1852,13 +2268,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Feuil1">
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
+  <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2074,10 +2488,10 @@
     </row>
     <row r="19" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="78"/>
-      <c r="B19" s="98" t="s">
+      <c r="B19" s="146" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="99"/>
+      <c r="C19" s="147"/>
       <c r="D19" s="59"/>
       <c r="E19" s="59"/>
       <c r="F19" s="59"/>
@@ -2141,7 +2555,7 @@
         <v>4</v>
       </c>
       <c r="C24" s="70" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D24" s="59"/>
       <c r="E24" s="59"/>
@@ -2154,7 +2568,7 @@
         <v>5</v>
       </c>
       <c r="C25" s="70" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D25" s="59"/>
       <c r="E25" s="59"/>
@@ -2167,7 +2581,7 @@
         <v>6</v>
       </c>
       <c r="C26" s="70" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D26" s="59"/>
       <c r="E26" s="59"/>
@@ -2180,7 +2594,7 @@
         <v>7</v>
       </c>
       <c r="C27" s="70" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D27" s="59"/>
       <c r="E27" s="59"/>
@@ -2193,7 +2607,7 @@
         <v>8</v>
       </c>
       <c r="C28" s="71" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D28" s="59"/>
       <c r="E28" s="59"/>
@@ -2206,7 +2620,7 @@
         <v>9</v>
       </c>
       <c r="C29" s="71" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D29" s="59"/>
       <c r="E29" s="59"/>
@@ -2219,7 +2633,7 @@
         <v>10</v>
       </c>
       <c r="C30" s="70" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D30" s="59"/>
       <c r="E30" s="59"/>
@@ -2232,7 +2646,7 @@
         <v>11</v>
       </c>
       <c r="C31" s="70" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D31" s="59"/>
       <c r="E31" s="59"/>
@@ -2245,7 +2659,7 @@
         <v>12</v>
       </c>
       <c r="C32" s="70" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D32" s="59"/>
       <c r="E32" s="59"/>
@@ -2258,7 +2672,7 @@
         <v>13</v>
       </c>
       <c r="C33" s="70" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D33" s="59"/>
       <c r="E33" s="59"/>
@@ -2271,7 +2685,7 @@
         <v>14</v>
       </c>
       <c r="C34" s="71" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D34" s="59"/>
       <c r="E34" s="59"/>
@@ -2283,8 +2697,8 @@
       <c r="B35" s="81">
         <v>15</v>
       </c>
-      <c r="C35" s="71" t="s">
-        <v>62</v>
+      <c r="C35" s="70" t="s">
+        <v>72</v>
       </c>
       <c r="D35" s="59"/>
       <c r="E35" s="59"/>
@@ -2296,7 +2710,9 @@
       <c r="B36" s="79">
         <v>16</v>
       </c>
-      <c r="C36" s="70"/>
+      <c r="C36" s="70" t="s">
+        <v>68</v>
+      </c>
       <c r="D36" s="59"/>
       <c r="E36" s="59"/>
       <c r="F36" s="59"/>
@@ -2489,7 +2905,7 @@
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="52" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="50" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"ETML L,Normal"ETML&amp;C&amp;"-,Normal"Planification&amp;R&amp;G</oddHeader>
     <oddFooter>&amp;L&amp;"-,Normal"&amp;D - GGZ&amp;C&amp;"-,Normal"&amp;F - &amp;A&amp;R&amp;"-,Normal"Page &amp;P/&amp;N</oddFooter>
@@ -2609,7 +3025,7 @@
     </row>
     <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
-      <c r="B3" s="100" t="s">
+      <c r="B3" s="148" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="16">
@@ -2618,7 +3034,7 @@
     </row>
     <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
-      <c r="B4" s="101"/>
+      <c r="B4" s="149"/>
       <c r="C4" s="22">
         <v>0</v>
       </c>
@@ -3277,10 +3693,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{080FAF2F-C534-499F-8C25-95E6F074E70C}">
   <sheetPr codeName="Feuil9"/>
-  <dimension ref="A1:H154"/>
+  <dimension ref="A1:H147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -3308,70 +3724,50 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="115" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="116" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="115" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="115" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="52" customFormat="1" ht="54" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="4">
-        <v>2</v>
-      </c>
-      <c r="C3" s="88" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="9"/>
-    </row>
-    <row r="4" spans="1:4" s="52" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" s="89" t="s">
-        <v>57</v>
-      </c>
-      <c r="D4" s="10"/>
-    </row>
-    <row r="5" spans="1:4" s="52" customFormat="1" ht="127.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="2">
-        <v>5</v>
-      </c>
-      <c r="C5" s="89" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" s="93" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="52" customFormat="1" ht="54" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="2">
-        <v>1</v>
-      </c>
-      <c r="C6" s="89" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>37</v>
-      </c>
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="101"/>
+      <c r="B3" s="102"/>
+      <c r="C3" s="103" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="103"/>
+    </row>
+    <row r="4" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="97" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="98">
+        <v>9</v>
+      </c>
+      <c r="C4" s="99" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="100"/>
+    </row>
+    <row r="5" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="89"/>
+      <c r="D5" s="10"/>
+    </row>
+    <row r="6" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
     </row>
     <row r="7" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
@@ -3398,7 +3794,7 @@
       <c r="D10" s="10"/>
     </row>
     <row r="11" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -3416,10 +3812,10 @@
       <c r="D13" s="10"/>
     </row>
     <row r="14" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
+      <c r="A14" s="50"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
     </row>
     <row r="15" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="50"/>
@@ -3427,152 +3823,117 @@
       <c r="C15" s="51"/>
       <c r="D15" s="51"/>
     </row>
-    <row r="16" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="50"/>
-      <c r="B16" s="50"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="51"/>
-    </row>
-    <row r="17" spans="1:8" s="52" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-    </row>
-    <row r="18" spans="1:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="47" t="s">
+    <row r="16" spans="1:4" s="52" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+    </row>
+    <row r="17" spans="1:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="47">
-        <f>SUM(B3:B17)</f>
+      <c r="B17" s="47">
+        <f>SUM(B3:B16)</f>
         <v>9</v>
       </c>
-      <c r="C18" s="87" t="s">
+      <c r="C17" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="48"/>
-    </row>
-    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="49"/>
-      <c r="B19" s="49"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-    </row>
-    <row r="20" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="42" t="s">
+      <c r="D17" s="48"/>
+    </row>
+    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="49"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+    </row>
+    <row r="19" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="43">
+      <c r="B19" s="43">
         <v>2</v>
       </c>
-      <c r="C20" s="44" t="s">
+      <c r="C19" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="53">
+      <c r="D19" s="53">
         <f>$D$1+7</f>
         <v>45971</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="45" t="s">
+    <row r="20" spans="1:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="46" t="s">
+      <c r="B20" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="45" t="s">
+      <c r="C20" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="45" t="s">
+      <c r="D20" s="45" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="96"/>
-      <c r="B22" s="97"/>
-      <c r="C22" s="96" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="96"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="4">
-        <v>1</v>
-      </c>
-      <c r="C23" s="88" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="54" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" s="2">
-        <v>1</v>
-      </c>
-      <c r="C24" s="89" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24" s="10"/>
-    </row>
-    <row r="25" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B25" s="2">
-        <v>2</v>
-      </c>
-      <c r="C25" s="95" t="s">
-        <v>54</v>
-      </c>
+    <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="96"/>
+      <c r="B21" s="95"/>
+      <c r="C21" s="94" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="94"/>
+    </row>
+    <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="111"/>
+      <c r="B22" s="112"/>
+      <c r="C22" s="113"/>
+      <c r="D22" s="114"/>
+    </row>
+    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="107"/>
+      <c r="B23" s="108"/>
+      <c r="C23" s="109"/>
+      <c r="D23" s="110"/>
+    </row>
+    <row r="24" spans="1:8" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="97"/>
+      <c r="B24" s="105"/>
+      <c r="C24" s="106"/>
+      <c r="D24" s="106"/>
+    </row>
+    <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="93"/>
       <c r="D25" s="10"/>
-    </row>
-    <row r="26" spans="1:8" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B26" s="2">
-        <v>1</v>
-      </c>
-      <c r="C26" s="95" t="s">
-        <v>45</v>
-      </c>
+      <c r="F25" s="34"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="93"/>
       <c r="D26" s="10"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="33"/>
-    </row>
-    <row r="27" spans="1:8" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B27" s="2">
-        <v>2</v>
-      </c>
-      <c r="C27" s="95" t="s">
-        <v>48</v>
-      </c>
+      <c r="F26" s="36"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="10"/>
       <c r="D27" s="10"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="30"/>
-    </row>
-    <row r="28" spans="1:8" ht="27" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="2">
-        <v>2</v>
-      </c>
-      <c r="C28" s="95" t="s">
-        <v>53</v>
-      </c>
+      <c r="F27" s="36"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="10"/>
       <c r="D28" s="10"/>
       <c r="F28" s="36"/>
       <c r="G28" s="37"/>
@@ -3588,7 +3949,7 @@
       <c r="H29" s="37"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
+      <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
@@ -3597,7 +3958,7 @@
       <c r="H30" s="37"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
+      <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
@@ -3615,292 +3976,320 @@
       <c r="H32" s="37"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
+      <c r="A33" s="50"/>
+      <c r="B33" s="50"/>
+      <c r="C33" s="51"/>
+      <c r="D33" s="51"/>
       <c r="F33" s="36"/>
       <c r="G33" s="37"/>
       <c r="H33" s="37"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="37"/>
-      <c r="H34" s="37"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="50"/>
-      <c r="B35" s="50"/>
-      <c r="C35" s="51"/>
-      <c r="D35" s="51"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="37"/>
-      <c r="H35" s="37"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="50"/>
-      <c r="B36" s="50"/>
-      <c r="C36" s="51"/>
-      <c r="D36" s="51"/>
-      <c r="F36" s="38"/>
-      <c r="G36" s="39"/>
-      <c r="H36" s="39"/>
+      <c r="A34" s="50"/>
+      <c r="B34" s="50"/>
+      <c r="C34" s="51"/>
+      <c r="D34" s="51"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="39"/>
+      <c r="H34" s="39"/>
+    </row>
+    <row r="35" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="F35" s="40"/>
+      <c r="G35" s="40"/>
+      <c r="H35" s="40"/>
+    </row>
+    <row r="36" spans="1:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" s="47">
+        <f>SUM(B22:B35)</f>
+        <v>0</v>
+      </c>
+      <c r="C36" s="87" t="s">
+        <v>28</v>
+      </c>
+      <c r="D36" s="48"/>
     </row>
     <row r="37" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="F37" s="40"/>
-      <c r="G37" s="40"/>
-      <c r="H37" s="40"/>
-    </row>
-    <row r="38" spans="1:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="47" t="s">
+      <c r="A37" s="49"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49"/>
+    </row>
+    <row r="38" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="129">
+        <v>3</v>
+      </c>
+      <c r="C38" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="D38" s="143">
+        <f>$D$19+7</f>
+        <v>45978</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="121" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" s="130" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="135" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="115" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="54" x14ac:dyDescent="0.25">
+      <c r="A40" s="122" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40" s="112">
+        <v>2</v>
+      </c>
+      <c r="C40" s="134" t="s">
+        <v>69</v>
+      </c>
+      <c r="D40" s="118"/>
+    </row>
+    <row r="41" spans="1:8" ht="27" x14ac:dyDescent="0.25">
+      <c r="A41" s="120" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41" s="112">
+        <v>1</v>
+      </c>
+      <c r="C41" s="136" t="s">
+        <v>51</v>
+      </c>
+      <c r="D41" s="119"/>
+    </row>
+    <row r="42" spans="1:8" ht="162" x14ac:dyDescent="0.25">
+      <c r="A42" s="133" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42" s="112">
+        <v>5</v>
+      </c>
+      <c r="C42" s="113" t="s">
+        <v>61</v>
+      </c>
+      <c r="D42" s="113" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="54" x14ac:dyDescent="0.25">
+      <c r="A43" s="111" t="s">
+        <v>34</v>
+      </c>
+      <c r="B43" s="112">
+        <v>1</v>
+      </c>
+      <c r="C43" s="145" t="s">
+        <v>35</v>
+      </c>
+      <c r="D43" s="113"/>
+    </row>
+    <row r="44" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="123"/>
+      <c r="B44" s="117"/>
+      <c r="C44" s="137" t="s">
+        <v>62</v>
+      </c>
+      <c r="D44" s="119"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="124" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45" s="131">
+        <v>9</v>
+      </c>
+      <c r="C45" s="138" t="s">
+        <v>60</v>
+      </c>
+      <c r="D45" s="10"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="124"/>
+      <c r="B46" s="131"/>
+      <c r="C46" s="139"/>
+      <c r="D46" s="10"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="125"/>
+      <c r="B47" s="131"/>
+      <c r="C47" s="139"/>
+      <c r="D47" s="10"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="125"/>
+      <c r="B48" s="131"/>
+      <c r="C48" s="139"/>
+      <c r="D48" s="10"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="125"/>
+      <c r="B49" s="131"/>
+      <c r="C49" s="139"/>
+      <c r="D49" s="10"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="126"/>
+      <c r="B50" s="131"/>
+      <c r="C50" s="140"/>
+      <c r="D50" s="51"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="126"/>
+      <c r="B51" s="131"/>
+      <c r="C51" s="140"/>
+      <c r="D51" s="51"/>
+    </row>
+    <row r="52" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="127"/>
+      <c r="B52" s="131"/>
+      <c r="C52" s="141"/>
+      <c r="D52" s="11"/>
+    </row>
+    <row r="53" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="128" t="s">
         <v>22</v>
       </c>
-      <c r="B38" s="47">
-        <f>SUM(B23:B37)</f>
-        <v>9</v>
-      </c>
-      <c r="C38" s="87" t="s">
-        <v>28</v>
-      </c>
-      <c r="D38" s="48"/>
-    </row>
-    <row r="39" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="49"/>
-      <c r="B39" s="49"/>
-      <c r="C39" s="49"/>
-      <c r="D39" s="49"/>
-    </row>
-    <row r="40" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="42" t="s">
+      <c r="B53" s="132">
+        <f>SUM(B40:B52)</f>
+        <v>18</v>
+      </c>
+      <c r="C53" s="142" t="s">
+        <v>63</v>
+      </c>
+      <c r="D53" s="144"/>
+    </row>
+    <row r="54" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="49"/>
+      <c r="B54" s="49"/>
+      <c r="C54" s="49"/>
+      <c r="D54" s="49"/>
+    </row>
+    <row r="55" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B40" s="43">
+      <c r="B55" s="43">
+        <v>4</v>
+      </c>
+      <c r="C55" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="D55" s="53">
+        <f>$D$38+7</f>
+        <v>45985</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="C40" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="D40" s="53">
-        <f>$D$20+7</f>
-        <v>45978</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="B41" s="46" t="s">
+      <c r="B56" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C41" s="45" t="s">
+      <c r="C56" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D41" s="45" t="s">
+      <c r="D56" s="45" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="27" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B42" s="4">
+    <row r="57" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="5"/>
+      <c r="B57" s="95"/>
+      <c r="C57" s="103" t="s">
+        <v>45</v>
+      </c>
+      <c r="D57" s="94"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B58" s="4">
+        <v>1</v>
+      </c>
+      <c r="C58" s="88" t="s">
+        <v>38</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="54" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B59" s="2">
+        <v>1</v>
+      </c>
+      <c r="C59" s="89" t="s">
+        <v>50</v>
+      </c>
+      <c r="D59" s="10"/>
+    </row>
+    <row r="60" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B60" s="2">
         <v>2</v>
       </c>
-      <c r="C42" s="95" t="s">
-        <v>52</v>
-      </c>
-      <c r="D42" s="9"/>
-    </row>
-    <row r="43" spans="1:8" ht="27" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B43" s="2">
+      <c r="C60" s="89" t="s">
+        <v>73</v>
+      </c>
+      <c r="D60" s="10"/>
+    </row>
+    <row r="61" spans="1:4" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B61" s="2">
         <v>1</v>
       </c>
-      <c r="C43" s="95" t="s">
-        <v>51</v>
-      </c>
-      <c r="D43" s="10"/>
-    </row>
-    <row r="44" spans="1:8" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B44" s="2">
-        <v>1</v>
-      </c>
-      <c r="C44" s="95" t="s">
-        <v>63</v>
-      </c>
-      <c r="D44" s="10"/>
-    </row>
-    <row r="45" spans="1:8" ht="54" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B45" s="2">
+      <c r="C61" s="89" t="s">
+        <v>43</v>
+      </c>
+      <c r="D61" s="10"/>
+    </row>
+    <row r="62" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B62" s="2">
         <v>2</v>
       </c>
-      <c r="C45" s="95" t="s">
-        <v>64</v>
-      </c>
-      <c r="D45" s="10"/>
-    </row>
-    <row r="46" spans="1:8" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B46" s="2">
+      <c r="C62" s="89" t="s">
+        <v>74</v>
+      </c>
+      <c r="D62" s="10"/>
+    </row>
+    <row r="63" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B63" s="2">
         <v>2</v>
       </c>
-      <c r="C46" s="95" t="s">
-        <v>65</v>
-      </c>
-      <c r="D46" s="10"/>
-    </row>
-    <row r="47" spans="1:8" ht="27" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B47" s="2">
-        <v>1</v>
-      </c>
-      <c r="C47" s="95" t="s">
-        <v>66</v>
-      </c>
-      <c r="D47" s="10"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="2"/>
-      <c r="B51" s="2"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="10"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="2"/>
-      <c r="B53" s="2"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="50"/>
-      <c r="B54" s="50"/>
-      <c r="C54" s="51"/>
-      <c r="D54" s="51"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="50"/>
-      <c r="B55" s="50"/>
-      <c r="C55" s="51"/>
-      <c r="D55" s="51"/>
-    </row>
-    <row r="56" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="3"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="11"/>
-      <c r="D56" s="11"/>
-    </row>
-    <row r="57" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="47" t="s">
-        <v>22</v>
-      </c>
-      <c r="B57" s="47">
-        <f>SUM(B42:B56)</f>
-        <v>9</v>
-      </c>
-      <c r="C57" s="87" t="s">
-        <v>28</v>
-      </c>
-      <c r="D57" s="48"/>
-    </row>
-    <row r="58" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="49"/>
-      <c r="B58" s="49"/>
-      <c r="C58" s="49"/>
-      <c r="D58" s="49"/>
-    </row>
-    <row r="59" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="B59" s="43">
-        <v>4</v>
-      </c>
-      <c r="C59" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="D59" s="53">
-        <f>$D$40+7</f>
-        <v>45985</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="B60" s="46" t="s">
-        <v>15</v>
-      </c>
-      <c r="C60" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="D60" s="45" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B61" s="4"/>
-      <c r="C61" s="88"/>
-      <c r="D61" s="90"/>
-    </row>
-    <row r="62" spans="1:4" ht="27" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B62" s="2"/>
-      <c r="C62" s="10"/>
-      <c r="D62" s="10"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
-      <c r="B63" s="2"/>
-      <c r="C63" s="10"/>
+      <c r="C63" s="89" t="s">
+        <v>75</v>
+      </c>
       <c r="D63" s="10"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -3910,129 +4299,167 @@
       <c r="D64" s="10"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
+      <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="10"/>
       <c r="D65" s="10"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
+      <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="10"/>
       <c r="D66" s="10"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
+      <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="10"/>
       <c r="D67" s="10"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
-      <c r="B68" s="2"/>
-      <c r="C68" s="10"/>
-      <c r="D68" s="10"/>
+      <c r="A68" s="50"/>
+      <c r="B68" s="50"/>
+      <c r="C68" s="51"/>
+      <c r="D68" s="51"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="1"/>
-      <c r="B69" s="2"/>
-      <c r="C69" s="10"/>
-      <c r="D69" s="10"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="2"/>
-      <c r="B70" s="2"/>
-      <c r="C70" s="10"/>
-      <c r="D70" s="10"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="2"/>
-      <c r="B71" s="2"/>
-      <c r="C71" s="10"/>
-      <c r="D71" s="10"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="2"/>
-      <c r="B72" s="2"/>
-      <c r="C72" s="10"/>
-      <c r="D72" s="10"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="50"/>
-      <c r="B73" s="50"/>
-      <c r="C73" s="51"/>
-      <c r="D73" s="51"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="50"/>
-      <c r="B74" s="50"/>
-      <c r="C74" s="51"/>
-      <c r="D74" s="51"/>
-    </row>
-    <row r="75" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="3"/>
-      <c r="B75" s="3"/>
-      <c r="C75" s="11"/>
-      <c r="D75" s="11"/>
-    </row>
-    <row r="76" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="47" t="s">
+      <c r="A69" s="50"/>
+      <c r="B69" s="50"/>
+      <c r="C69" s="51"/>
+      <c r="D69" s="51"/>
+    </row>
+    <row r="70" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="3"/>
+      <c r="B70" s="3"/>
+      <c r="C70" s="11"/>
+      <c r="D70" s="11"/>
+    </row>
+    <row r="71" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B76" s="47">
-        <f>SUM(B61:B75)</f>
-        <v>0</v>
-      </c>
-      <c r="C76" s="87" t="s">
+      <c r="B71" s="47">
+        <f>SUM(B57:B70)</f>
+        <v>9</v>
+      </c>
+      <c r="C71" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="D76" s="48"/>
-    </row>
-    <row r="77" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="49"/>
-      <c r="B77" s="49"/>
-      <c r="C77" s="49"/>
-      <c r="D77" s="49"/>
-    </row>
-    <row r="78" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="42" t="s">
+      <c r="D71" s="48"/>
+    </row>
+    <row r="72" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="49"/>
+      <c r="B72" s="49"/>
+      <c r="C72" s="49"/>
+      <c r="D72" s="49"/>
+    </row>
+    <row r="73" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B78" s="43">
+      <c r="B73" s="43">
         <v>5</v>
       </c>
-      <c r="C78" s="44" t="s">
+      <c r="C73" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="D78" s="53">
-        <f>$D$59+7</f>
+      <c r="D73" s="53">
+        <f>$D$55+7</f>
         <v>45992</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="45" t="s">
+    <row r="74" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B79" s="46" t="s">
+      <c r="B74" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C79" s="45" t="s">
+      <c r="C74" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D79" s="45" t="s">
+      <c r="D74" s="45" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="5"/>
-      <c r="B80" s="4"/>
-      <c r="C80" s="88"/>
-      <c r="D80" s="9"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="1"/>
-      <c r="B81" s="2"/>
-      <c r="C81" s="10"/>
+    <row r="75" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="5"/>
+      <c r="B75" s="95"/>
+      <c r="C75" s="103" t="s">
+        <v>67</v>
+      </c>
+      <c r="D75" s="94"/>
+    </row>
+    <row r="76" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A76" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B76" s="4">
+        <v>2</v>
+      </c>
+      <c r="C76" s="99" t="s">
+        <v>49</v>
+      </c>
+      <c r="D76" s="10"/>
+    </row>
+    <row r="77" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B77" s="2">
+        <v>1</v>
+      </c>
+      <c r="C77" s="89" t="s">
+        <v>48</v>
+      </c>
+      <c r="D77" s="10"/>
+    </row>
+    <row r="78" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B78" s="2">
+        <v>1</v>
+      </c>
+      <c r="C78" s="89" t="s">
+        <v>56</v>
+      </c>
+      <c r="D78" s="10"/>
+    </row>
+    <row r="79" spans="1:4" ht="54" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B79" s="2">
+        <v>2</v>
+      </c>
+      <c r="C79" s="89" t="s">
+        <v>57</v>
+      </c>
+      <c r="D79" s="10"/>
+    </row>
+    <row r="80" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B80" s="2">
+        <v>2</v>
+      </c>
+      <c r="C80" s="89" t="s">
+        <v>58</v>
+      </c>
+      <c r="D80" s="10"/>
+    </row>
+    <row r="81" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B81" s="2">
+        <v>1</v>
+      </c>
+      <c r="C81" s="89" t="s">
+        <v>59</v>
+      </c>
       <c r="D81" s="10"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -4048,528 +4475,508 @@
       <c r="D83" s="10"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="1"/>
+      <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="10"/>
       <c r="D84" s="10"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="1"/>
+      <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="10"/>
       <c r="D85" s="10"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="1"/>
+      <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="10"/>
       <c r="D86" s="10"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="1"/>
-      <c r="B87" s="2"/>
-      <c r="C87" s="10"/>
-      <c r="D87" s="10"/>
+      <c r="A87" s="50"/>
+      <c r="B87" s="50"/>
+      <c r="C87" s="51"/>
+      <c r="D87" s="51"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="1"/>
-      <c r="B88" s="2"/>
-      <c r="C88" s="10"/>
-      <c r="D88" s="10"/>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="2"/>
-      <c r="B89" s="2"/>
-      <c r="C89" s="10"/>
-      <c r="D89" s="10"/>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="2"/>
-      <c r="B90" s="2"/>
-      <c r="C90" s="10"/>
-      <c r="D90" s="10"/>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="2"/>
-      <c r="B91" s="2"/>
-      <c r="C91" s="10"/>
-      <c r="D91" s="10"/>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="50"/>
-      <c r="B92" s="50"/>
-      <c r="C92" s="51"/>
-      <c r="D92" s="51"/>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="50"/>
-      <c r="B93" s="50"/>
-      <c r="C93" s="51"/>
-      <c r="D93" s="51"/>
-    </row>
-    <row r="94" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="3"/>
-      <c r="B94" s="3"/>
-      <c r="C94" s="11"/>
-      <c r="D94" s="11"/>
-    </row>
-    <row r="95" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="47" t="s">
+      <c r="A88" s="50"/>
+      <c r="B88" s="50"/>
+      <c r="C88" s="51"/>
+      <c r="D88" s="51"/>
+    </row>
+    <row r="89" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="3"/>
+      <c r="B89" s="3"/>
+      <c r="C89" s="11"/>
+      <c r="D89" s="11"/>
+    </row>
+    <row r="90" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B95" s="47">
-        <f>SUM(B80:B94)</f>
-        <v>0</v>
-      </c>
-      <c r="C95" s="87" t="s">
+      <c r="B90" s="47">
+        <f>SUM(B75:B89)</f>
+        <v>9</v>
+      </c>
+      <c r="C90" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="D95" s="48"/>
-    </row>
-    <row r="96" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="49"/>
-      <c r="B96" s="49"/>
-      <c r="C96" s="49"/>
-      <c r="D96" s="49"/>
-    </row>
-    <row r="97" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="42" t="s">
+      <c r="D90" s="48"/>
+    </row>
+    <row r="91" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A91" s="49"/>
+      <c r="B91" s="49"/>
+      <c r="C91" s="49"/>
+      <c r="D91" s="49"/>
+    </row>
+    <row r="92" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B97" s="43">
+      <c r="B92" s="43">
         <v>6</v>
       </c>
-      <c r="C97" s="44" t="s">
+      <c r="C92" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="D97" s="53">
-        <f>$D$78+7</f>
+      <c r="D92" s="53">
+        <f>$D$73+7</f>
         <v>45999</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="45" t="s">
+    <row r="93" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B98" s="46" t="s">
+      <c r="B93" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C98" s="45" t="s">
+      <c r="C93" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D98" s="45" t="s">
+      <c r="D93" s="45" t="s">
         <v>13</v>
       </c>
     </row>
+    <row r="94" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="101"/>
+      <c r="B94" s="102"/>
+      <c r="C94" s="103" t="s">
+        <v>66</v>
+      </c>
+      <c r="D94" s="103"/>
+    </row>
+    <row r="95" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A95" s="97" t="s">
+        <v>68</v>
+      </c>
+      <c r="B95" s="98">
+        <v>3</v>
+      </c>
+      <c r="C95" s="89" t="s">
+        <v>70</v>
+      </c>
+      <c r="D95" s="104"/>
+    </row>
+    <row r="96" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B96" s="2">
+        <v>3</v>
+      </c>
+      <c r="C96" s="89" t="s">
+        <v>71</v>
+      </c>
+      <c r="D96" s="10"/>
+    </row>
+    <row r="97" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B97" s="2">
+        <v>3</v>
+      </c>
+      <c r="C97" s="93" t="s">
+        <v>76</v>
+      </c>
+      <c r="D97" s="10"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B98" s="2"/>
+      <c r="C98" s="10"/>
+      <c r="D98" s="10"/>
+    </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="5"/>
-      <c r="B99" s="4"/>
-      <c r="C99" s="88"/>
-      <c r="D99" s="91"/>
+      <c r="A99" s="1"/>
+      <c r="B99" s="2"/>
+      <c r="C99" s="10"/>
+      <c r="D99" s="10"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
-      <c r="C100" s="89"/>
-      <c r="D100" s="93"/>
+      <c r="C100" s="10"/>
+      <c r="D100" s="10"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="1"/>
+      <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="10"/>
       <c r="D101" s="10"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="1"/>
+      <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="10"/>
       <c r="D102" s="10"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="1"/>
+      <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="10"/>
       <c r="D103" s="10"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="1"/>
-      <c r="B104" s="2"/>
-      <c r="C104" s="10"/>
-      <c r="D104" s="10"/>
+      <c r="A104" s="50"/>
+      <c r="B104" s="50"/>
+      <c r="C104" s="51"/>
+      <c r="D104" s="51"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="1"/>
-      <c r="B105" s="2"/>
-      <c r="C105" s="10"/>
-      <c r="D105" s="10"/>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="1"/>
-      <c r="B106" s="2"/>
-      <c r="C106" s="10"/>
-      <c r="D106" s="10"/>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="1"/>
-      <c r="B107" s="2"/>
-      <c r="C107" s="10"/>
-      <c r="D107" s="10"/>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="2"/>
-      <c r="B108" s="2"/>
-      <c r="C108" s="10"/>
-      <c r="D108" s="10"/>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="2"/>
-      <c r="B109" s="2"/>
-      <c r="C109" s="10"/>
-      <c r="D109" s="10"/>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="2"/>
-      <c r="B110" s="2"/>
-      <c r="C110" s="10"/>
-      <c r="D110" s="10"/>
+      <c r="A105" s="50"/>
+      <c r="B105" s="50"/>
+      <c r="C105" s="51"/>
+      <c r="D105" s="51"/>
+    </row>
+    <row r="106" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="3"/>
+      <c r="B106" s="3"/>
+      <c r="C106" s="11"/>
+      <c r="D106" s="11"/>
+    </row>
+    <row r="107" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="B107" s="47">
+        <f>SUM(B94:B106)</f>
+        <v>9</v>
+      </c>
+      <c r="C107" s="87" t="s">
+        <v>28</v>
+      </c>
+      <c r="D107" s="48"/>
+    </row>
+    <row r="108" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A108" s="49"/>
+      <c r="B108" s="49"/>
+      <c r="C108" s="49"/>
+      <c r="D108" s="49"/>
+    </row>
+    <row r="109" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B109" s="43">
+        <v>7</v>
+      </c>
+      <c r="C109" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="D109" s="53">
+        <f>$D$92+7</f>
+        <v>46006</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="B110" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="C110" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="D110" s="45" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="50"/>
-      <c r="B111" s="50"/>
-      <c r="C111" s="51"/>
-      <c r="D111" s="51"/>
+      <c r="A111" s="5"/>
+      <c r="B111" s="4"/>
+      <c r="C111" s="88"/>
+      <c r="D111" s="9"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="50"/>
-      <c r="B112" s="50"/>
-      <c r="C112" s="51"/>
-      <c r="D112" s="51"/>
-    </row>
-    <row r="113" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="3"/>
-      <c r="B113" s="3"/>
-      <c r="C113" s="11"/>
-      <c r="D113" s="11"/>
-    </row>
-    <row r="114" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="47" t="s">
-        <v>22</v>
-      </c>
-      <c r="B114" s="47">
-        <f>SUM(B99:B113)</f>
-        <v>0</v>
-      </c>
-      <c r="C114" s="87" t="s">
-        <v>28</v>
-      </c>
-      <c r="D114" s="48"/>
-    </row>
-    <row r="115" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A115" s="49"/>
-      <c r="B115" s="49"/>
-      <c r="C115" s="49"/>
-      <c r="D115" s="49"/>
-    </row>
-    <row r="116" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="B116" s="43">
-        <v>7</v>
-      </c>
-      <c r="C116" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="D116" s="53">
-        <f>$D$97+7</f>
-        <v>46006</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="B117" s="46" t="s">
-        <v>15</v>
-      </c>
-      <c r="C117" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="D117" s="45" t="s">
-        <v>13</v>
-      </c>
+      <c r="A112" s="1"/>
+      <c r="B112" s="2"/>
+      <c r="C112" s="90"/>
+      <c r="D112" s="10"/>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="1"/>
+      <c r="B113" s="2"/>
+      <c r="C113" s="89"/>
+      <c r="D113" s="91"/>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="1"/>
+      <c r="B114" s="2"/>
+      <c r="C114" s="10"/>
+      <c r="D114" s="10"/>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="1"/>
+      <c r="B115" s="2"/>
+      <c r="C115" s="10"/>
+      <c r="D115" s="10"/>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="1"/>
+      <c r="B116" s="2"/>
+      <c r="C116" s="10"/>
+      <c r="D116" s="10"/>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="1"/>
+      <c r="B117" s="2"/>
+      <c r="C117" s="10"/>
+      <c r="D117" s="10"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="5"/>
-      <c r="B118" s="4"/>
-      <c r="C118" s="88"/>
-      <c r="D118" s="9"/>
+      <c r="A118" s="1"/>
+      <c r="B118" s="2"/>
+      <c r="C118" s="10"/>
+      <c r="D118" s="10"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="2"/>
-      <c r="C119" s="92"/>
+      <c r="C119" s="10"/>
       <c r="D119" s="10"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="1"/>
+      <c r="A120" s="2"/>
       <c r="B120" s="2"/>
-      <c r="C120" s="89"/>
-      <c r="D120" s="93"/>
+      <c r="C120" s="10"/>
+      <c r="D120" s="10"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="1"/>
+      <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="10"/>
       <c r="D121" s="10"/>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="1"/>
+      <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="10"/>
       <c r="D122" s="10"/>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="1"/>
-      <c r="B123" s="2"/>
-      <c r="C123" s="10"/>
-      <c r="D123" s="10"/>
+      <c r="A123" s="50"/>
+      <c r="B123" s="50"/>
+      <c r="C123" s="51"/>
+      <c r="D123" s="51"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="1"/>
-      <c r="B124" s="2"/>
-      <c r="C124" s="10"/>
-      <c r="D124" s="10"/>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="1"/>
-      <c r="B125" s="2"/>
-      <c r="C125" s="10"/>
-      <c r="D125" s="10"/>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="1"/>
-      <c r="B126" s="2"/>
-      <c r="C126" s="10"/>
-      <c r="D126" s="10"/>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="2"/>
-      <c r="B127" s="2"/>
-      <c r="C127" s="10"/>
-      <c r="D127" s="10"/>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="2"/>
-      <c r="B128" s="2"/>
-      <c r="C128" s="10"/>
-      <c r="D128" s="10"/>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="2"/>
-      <c r="B129" s="2"/>
-      <c r="C129" s="10"/>
-      <c r="D129" s="10"/>
+      <c r="A124" s="50"/>
+      <c r="B124" s="50"/>
+      <c r="C124" s="51"/>
+      <c r="D124" s="51"/>
+    </row>
+    <row r="125" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="3"/>
+      <c r="B125" s="3"/>
+      <c r="C125" s="11"/>
+      <c r="D125" s="11"/>
+    </row>
+    <row r="126" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="B126" s="47">
+        <f>SUM(B111:B125)</f>
+        <v>0</v>
+      </c>
+      <c r="C126" s="87" t="s">
+        <v>30</v>
+      </c>
+      <c r="D126" s="48"/>
+    </row>
+    <row r="127" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A127" s="49"/>
+      <c r="B127" s="49"/>
+      <c r="C127" s="49"/>
+      <c r="D127" s="49"/>
+    </row>
+    <row r="128" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B128" s="43">
+        <v>8</v>
+      </c>
+      <c r="C128" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="D128" s="53">
+        <f>$D$109+21</f>
+        <v>46027</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="B129" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="C129" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="D129" s="45" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="50"/>
-      <c r="B130" s="50"/>
-      <c r="C130" s="51"/>
-      <c r="D130" s="51"/>
+      <c r="A130" s="5"/>
+      <c r="B130" s="4"/>
+      <c r="C130" s="92"/>
+      <c r="D130" s="9"/>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="50"/>
-      <c r="B131" s="50"/>
-      <c r="C131" s="51"/>
-      <c r="D131" s="51"/>
-    </row>
-    <row r="132" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="3"/>
-      <c r="B132" s="3"/>
-      <c r="C132" s="11"/>
-      <c r="D132" s="11"/>
-    </row>
-    <row r="133" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="47" t="s">
-        <v>22</v>
-      </c>
-      <c r="B133" s="47">
-        <f>SUM(B118:B132)</f>
-        <v>0</v>
-      </c>
-      <c r="C133" s="87" t="s">
-        <v>30</v>
-      </c>
-      <c r="D133" s="48"/>
-    </row>
-    <row r="134" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A134" s="49"/>
-      <c r="B134" s="49"/>
-      <c r="C134" s="49"/>
-      <c r="D134" s="49"/>
-    </row>
-    <row r="135" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="B135" s="43">
-        <v>8</v>
-      </c>
-      <c r="C135" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="D135" s="53">
-        <f>$D$116+21</f>
-        <v>46027</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="B136" s="46" t="s">
-        <v>15</v>
-      </c>
-      <c r="C136" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="D136" s="45" t="s">
-        <v>13</v>
-      </c>
+      <c r="A131" s="1"/>
+      <c r="B131" s="2"/>
+      <c r="C131" s="93"/>
+      <c r="D131" s="10"/>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="1"/>
+      <c r="B132" s="2"/>
+      <c r="C132" s="10"/>
+      <c r="D132" s="10"/>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="1"/>
+      <c r="B133" s="2"/>
+      <c r="C133" s="10"/>
+      <c r="D133" s="10"/>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="1"/>
+      <c r="B134" s="2"/>
+      <c r="C134" s="10"/>
+      <c r="D134" s="10"/>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="1"/>
+      <c r="B135" s="2"/>
+      <c r="C135" s="10"/>
+      <c r="D135" s="10"/>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="1"/>
+      <c r="B136" s="2"/>
+      <c r="C136" s="10"/>
+      <c r="D136" s="10"/>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="5"/>
-      <c r="B137" s="4"/>
-      <c r="C137" s="94"/>
-      <c r="D137" s="9"/>
+      <c r="A137" s="1"/>
+      <c r="B137" s="2"/>
+      <c r="C137" s="10"/>
+      <c r="D137" s="10"/>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
       <c r="B138" s="2"/>
-      <c r="C138" s="95"/>
+      <c r="C138" s="10"/>
       <c r="D138" s="10"/>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="1"/>
+      <c r="A139" s="2"/>
       <c r="B139" s="2"/>
       <c r="C139" s="10"/>
       <c r="D139" s="10"/>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="1"/>
+      <c r="A140" s="2"/>
       <c r="B140" s="2"/>
       <c r="C140" s="10"/>
       <c r="D140" s="10"/>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="1"/>
+      <c r="A141" s="2"/>
       <c r="B141" s="2"/>
       <c r="C141" s="10"/>
       <c r="D141" s="10"/>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="1"/>
-      <c r="B142" s="2"/>
-      <c r="C142" s="10"/>
-      <c r="D142" s="10"/>
+      <c r="A142" s="50"/>
+      <c r="B142" s="50"/>
+      <c r="C142" s="51"/>
+      <c r="D142" s="51"/>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="1"/>
-      <c r="B143" s="2"/>
-      <c r="C143" s="10"/>
-      <c r="D143" s="10"/>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="1"/>
-      <c r="B144" s="2"/>
-      <c r="C144" s="10"/>
-      <c r="D144" s="10"/>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="1"/>
-      <c r="B145" s="2"/>
-      <c r="C145" s="10"/>
-      <c r="D145" s="10"/>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="2"/>
-      <c r="B146" s="2"/>
-      <c r="C146" s="10"/>
-      <c r="D146" s="10"/>
+      <c r="A143" s="50"/>
+      <c r="B143" s="50"/>
+      <c r="C143" s="51"/>
+      <c r="D143" s="51"/>
+    </row>
+    <row r="144" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A144" s="3"/>
+      <c r="B144" s="3"/>
+      <c r="C144" s="11"/>
+      <c r="D144" s="11"/>
+    </row>
+    <row r="145" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A145" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="B145" s="47">
+        <f>SUM(B130:B144)</f>
+        <v>0</v>
+      </c>
+      <c r="C145" s="87" t="s">
+        <v>28</v>
+      </c>
+      <c r="D145" s="48"/>
+    </row>
+    <row r="146" spans="1:4" ht="14.25" x14ac:dyDescent="0.3">
+      <c r="A146" s="49"/>
+      <c r="B146" s="49"/>
+      <c r="C146" s="49"/>
+      <c r="D146" s="49"/>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="2"/>
-      <c r="B147" s="2"/>
-      <c r="C147" s="10"/>
-      <c r="D147" s="10"/>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="2"/>
-      <c r="B148" s="2"/>
-      <c r="C148" s="10"/>
-      <c r="D148" s="10"/>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="50"/>
-      <c r="B149" s="50"/>
-      <c r="C149" s="51"/>
-      <c r="D149" s="51"/>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="50"/>
-      <c r="B150" s="50"/>
-      <c r="C150" s="51"/>
-      <c r="D150" s="51"/>
-    </row>
-    <row r="151" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A151" s="3"/>
-      <c r="B151" s="3"/>
-      <c r="C151" s="11"/>
-      <c r="D151" s="11"/>
-    </row>
-    <row r="152" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A152" s="47" t="s">
-        <v>22</v>
-      </c>
-      <c r="B152" s="47">
-        <f>SUM(B137:B151)</f>
-        <v>0</v>
-      </c>
-      <c r="C152" s="87" t="s">
-        <v>28</v>
-      </c>
-      <c r="D152" s="48"/>
-    </row>
-    <row r="153" spans="1:4" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A153" s="49"/>
-      <c r="B153" s="49"/>
-      <c r="C153" s="49"/>
-      <c r="D153" s="49"/>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="86" t="s">
+      <c r="A147" s="86" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="F36" xr:uid="{44460710-E505-40B8-8485-BA41A2FB3DB5}">
+    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="F34" xr:uid="{44460710-E505-40B8-8485-BA41A2FB3DB5}">
       <formula1>0</formula1>
       <formula2>DureePeriode-1</formula2>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="F28:F35 B3:B17 B23:B37 B42:B56 B61:B75 B80:B94 B99:B113 B118:B132 B137:B151" xr:uid="{B23B642E-0B29-4ED8-A409-C50EB7CC17BF}">
+    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="F26:F33 B45:B52 B4:B16 B76:B89 B111:B125 B130:B144 B25:B35 B58:B70 B95:B106" xr:uid="{B23B642E-0B29-4ED8-A409-C50EB7CC17BF}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B18 B38 B57 B76 B95 B114 B133 B152" xr:uid="{C02FA86D-12F2-40ED-8F5D-F7684A1E2EDD}">
+    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B17 B36 B53 B71 B90 B107 B126 B145" xr:uid="{C02FA86D-12F2-40ED-8F5D-F7684A1E2EDD}">
       <formula1>0</formula1>
       <formula2>NbPerWeek * NbQuartPer</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A17 A23:A37 A42:A56 A61:A75 A80:A94 A99:A113 A118:A132 A137:A151" xr:uid="{BCBC0613-73E6-47AF-B0DB-7981EF783ABA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A40:A52 A111:A125 A130:A144 A75:A89 A57:A70 A21:A35 A3:A16 A94:A106" xr:uid="{BCBC0613-73E6-47AF-B0DB-7981EF783ABA}">
       <formula1>lstTasks</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="80" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
   <controls>

</xml_diff>

<commit_message>
chore(documentation): ouverture des documents pour vérification
</commit_message>
<xml_diff>
--- a/T-P_App-MatiasDenis-JDT.xlsx
+++ b/T-P_App-MatiasDenis-JDT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\05-repertoires-ict-ssd (2022)\Deuxième année\P_App\P_App-Bruteforce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFEEA9C3-D9DD-495E-BCA1-D78D3595E508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D43573-833A-4DDB-8F36-AB98A537A64B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3695,7 +3695,7 @@
   <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:H147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
       <selection activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
doc(JdT, rapport, objectifs): documentation mise à jour
</commit_message>
<xml_diff>
--- a/T-P_App-MatiasDenis-JDT.xlsx
+++ b/T-P_App-MatiasDenis-JDT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\05-repertoires-ict-ssd (2022)\Deuxième année\P_App\P_App-Bruteforce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F59575-9AA5-4348-89B8-FCA26AE671C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8210AA-E95C-4300-A7E7-85E6C33982D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="86">
   <si>
     <t>Module :</t>
   </si>
@@ -158,9 +158,6 @@
     <t>STOP</t>
   </si>
   <si>
-    <t>Max. 15</t>
-  </si>
-  <si>
     <t>Choix du projet et prise de connaissance du CdC</t>
   </si>
   <si>
@@ -279,9 +276,6 @@
     <t>Jeudi 04.12</t>
   </si>
   <si>
-    <t>Mise au propre du journal de travail</t>
-  </si>
-  <si>
     <t>C'est le projet Bruteforce qui a été choisi. Le cahier des charges a été lu et compris. Tâche terminée.</t>
   </si>
   <si>
@@ -307,6 +301,44 @@
   </si>
   <si>
     <t>Lien à ajouter</t>
+  </si>
+  <si>
+    <t>Jeudi 18.12</t>
+  </si>
+  <si>
+    <t>Mise au propre du journal de travail avant impression</t>
+  </si>
+  <si>
+    <t>Modification de l'architecture du projet afin d'intégrer les protocoles SSH et HTTP via Docker</t>
+  </si>
+  <si>
+    <t>Adaptation et centralisation du code Python afin de gérer les différents protocoles de manière sécurisée</t>
+  </si>
+  <si>
+    <t>Mise en place et configuration des serveurs Docker (FTP, HTTP avec Basic Auth, SSH)</t>
+  </si>
+  <si>
+    <t>Tests et validation du fonctionnement global du projet</t>
+  </si>
+  <si>
+    <t>L’architecture du projet a été repensée afin d’intégrer plusieurs services réseau distincts.
+Chaque protocole (FTP, SSH et HTTP) est désormais déployé dans un conteneur Docker séparé, garantissant un environnement local, isolé et contrôlé.
+Cette approche permet de tester les mécanismes d’authentification sans interagir avec des services externes.</t>
+  </si>
+  <si>
+    <t>Le code Python a été restructuré pour être centralisé dans un seul fichier principal (bruteforce.py).
+Ce script permet de sélectionner différents modes de fonctionnement (FTP, HTTP ou SSH) tout en limitant strictement les connexions à l’environnement local.
+Cette centralisation améliore la lisibilité du code et réduit les risques d’erreurs ou d’utilisations non prévues.</t>
+  </si>
+  <si>
+    <t>Les serveurs FTP, HTTP et SSH ont été configurés à l’aide d’images Docker adaptées à chaque protocole.
+Le service HTTP est protégé par une authentification Basic Auth avec mot de passe hashé, tandis que le service SSH utilise une authentification par mot de passe configurée côté serveur.
+Les paramètres Docker ont été ajustés pour assurer la stabilité des services et le respect des consignes de sécurité.</t>
+  </si>
+  <si>
+    <t>Chaque service a été testé individuellement afin de vérifier son bon fonctionnement et son accessibilité locale.
+Le bruteforce FTP a été validé par la découverte du mot de passe, tandis que les services HTTP et SSH ont été vérifiés par des tests d’authentification et l’analyse des logs.
+Ces tests ont permis de confirmer que l’ensemble du projet fonctionne correctement et conformément aux objectifs définis.</t>
   </si>
 </sst>
 </file>
@@ -1166,7 +1198,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1417,10 +1449,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -2274,8 +2302,8 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A22" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2491,10 +2519,10 @@
     </row>
     <row r="19" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="78"/>
-      <c r="B19" s="146" t="s">
+      <c r="B19" s="145" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="147"/>
+      <c r="C19" s="146"/>
       <c r="D19" s="59"/>
       <c r="E19" s="59"/>
       <c r="F19" s="59"/>
@@ -2519,7 +2547,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="69" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D21" s="59"/>
       <c r="E21" s="59"/>
@@ -2532,7 +2560,7 @@
         <v>2</v>
       </c>
       <c r="C22" s="70" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D22" s="59"/>
       <c r="E22" s="59"/>
@@ -2545,7 +2573,7 @@
         <v>3</v>
       </c>
       <c r="C23" s="70" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D23" s="59"/>
       <c r="E23" s="59"/>
@@ -2558,7 +2586,7 @@
         <v>4</v>
       </c>
       <c r="C24" s="70" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D24" s="59"/>
       <c r="E24" s="59"/>
@@ -2571,7 +2599,7 @@
         <v>5</v>
       </c>
       <c r="C25" s="70" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D25" s="59"/>
       <c r="E25" s="59"/>
@@ -2584,7 +2612,7 @@
         <v>6</v>
       </c>
       <c r="C26" s="70" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D26" s="59"/>
       <c r="E26" s="59"/>
@@ -2597,7 +2625,7 @@
         <v>7</v>
       </c>
       <c r="C27" s="70" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D27" s="59"/>
       <c r="E27" s="59"/>
@@ -2610,7 +2638,7 @@
         <v>8</v>
       </c>
       <c r="C28" s="71" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D28" s="59"/>
       <c r="E28" s="59"/>
@@ -2623,7 +2651,7 @@
         <v>9</v>
       </c>
       <c r="C29" s="71" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D29" s="59"/>
       <c r="E29" s="59"/>
@@ -2636,7 +2664,7 @@
         <v>10</v>
       </c>
       <c r="C30" s="70" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D30" s="59"/>
       <c r="E30" s="59"/>
@@ -2649,7 +2677,7 @@
         <v>11</v>
       </c>
       <c r="C31" s="70" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D31" s="59"/>
       <c r="E31" s="59"/>
@@ -2662,7 +2690,7 @@
         <v>12</v>
       </c>
       <c r="C32" s="70" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D32" s="59"/>
       <c r="E32" s="59"/>
@@ -2675,7 +2703,7 @@
         <v>13</v>
       </c>
       <c r="C33" s="70" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D33" s="59"/>
       <c r="E33" s="59"/>
@@ -2688,7 +2716,7 @@
         <v>14</v>
       </c>
       <c r="C34" s="71" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D34" s="59"/>
       <c r="E34" s="59"/>
@@ -2701,7 +2729,7 @@
         <v>15</v>
       </c>
       <c r="C35" s="70" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D35" s="59"/>
       <c r="E35" s="59"/>
@@ -2714,7 +2742,7 @@
         <v>16</v>
       </c>
       <c r="C36" s="70" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="D36" s="59"/>
       <c r="E36" s="59"/>
@@ -2726,7 +2754,9 @@
       <c r="B37" s="79">
         <v>17</v>
       </c>
-      <c r="C37" s="70"/>
+      <c r="C37" s="70" t="s">
+        <v>78</v>
+      </c>
       <c r="D37" s="59"/>
       <c r="E37" s="59"/>
       <c r="F37" s="59"/>
@@ -2737,7 +2767,9 @@
       <c r="B38" s="81">
         <v>18</v>
       </c>
-      <c r="C38" s="70"/>
+      <c r="C38" s="71" t="s">
+        <v>79</v>
+      </c>
       <c r="D38" s="59"/>
       <c r="E38" s="59"/>
       <c r="F38" s="59"/>
@@ -2748,7 +2780,9 @@
       <c r="B39" s="79">
         <v>19</v>
       </c>
-      <c r="C39" s="70"/>
+      <c r="C39" s="70" t="s">
+        <v>80</v>
+      </c>
       <c r="D39" s="59"/>
       <c r="E39" s="59"/>
       <c r="F39" s="59"/>
@@ -2759,7 +2793,9 @@
       <c r="B40" s="79">
         <v>20</v>
       </c>
-      <c r="C40" s="71"/>
+      <c r="C40" s="71" t="s">
+        <v>81</v>
+      </c>
       <c r="D40" s="59"/>
       <c r="E40" s="59"/>
       <c r="F40" s="59"/>
@@ -2919,27 +2955,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2969,27 +3005,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -3028,7 +3064,7 @@
     </row>
     <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
-      <c r="B3" s="148" t="s">
+      <c r="B3" s="147" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="16">
@@ -3037,7 +3073,7 @@
     </row>
     <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
-      <c r="B4" s="149"/>
+      <c r="B4" s="148"/>
       <c r="C4" s="22">
         <v>0</v>
       </c>
@@ -3698,8 +3734,8 @@
   <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:H147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="D78" sqref="D78"/>
+    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
+      <selection activeCell="C117" sqref="C117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -3727,38 +3763,38 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="115" t="s">
+      <c r="A2" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="116" t="s">
+      <c r="B2" s="115" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="115" t="s">
+      <c r="C2" s="114" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="115" t="s">
+      <c r="D2" s="114" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="101"/>
-      <c r="B3" s="102"/>
-      <c r="C3" s="103" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="103"/>
+      <c r="A3" s="100"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="102" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="102"/>
     </row>
     <row r="4" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="97" t="s">
+      <c r="A4" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="98">
+      <c r="B4" s="97">
         <v>9</v>
       </c>
-      <c r="C4" s="99" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" s="100"/>
+      <c r="C4" s="98" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="99"/>
     </row>
     <row r="5" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -3881,35 +3917,35 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="96"/>
-      <c r="B21" s="95"/>
-      <c r="C21" s="94" t="s">
-        <v>65</v>
-      </c>
-      <c r="D21" s="94"/>
+      <c r="A21" s="95"/>
+      <c r="B21" s="94"/>
+      <c r="C21" s="93" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="93"/>
     </row>
     <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="111"/>
-      <c r="B22" s="112"/>
-      <c r="C22" s="113"/>
-      <c r="D22" s="114"/>
+      <c r="A22" s="110"/>
+      <c r="B22" s="111"/>
+      <c r="C22" s="112"/>
+      <c r="D22" s="113"/>
     </row>
     <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="107"/>
-      <c r="B23" s="108"/>
-      <c r="C23" s="109"/>
-      <c r="D23" s="110"/>
+      <c r="A23" s="106"/>
+      <c r="B23" s="107"/>
+      <c r="C23" s="108"/>
+      <c r="D23" s="109"/>
     </row>
     <row r="24" spans="1:8" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A24" s="97"/>
-      <c r="B24" s="105"/>
-      <c r="C24" s="106"/>
-      <c r="D24" s="106"/>
+      <c r="A24" s="96"/>
+      <c r="B24" s="104"/>
+      <c r="C24" s="105"/>
+      <c r="D24" s="105"/>
     </row>
     <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
-      <c r="C25" s="93"/>
+      <c r="C25" s="92"/>
       <c r="D25" s="10"/>
       <c r="F25" s="34"/>
       <c r="G25" s="30"/>
@@ -3918,7 +3954,7 @@
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
-      <c r="C26" s="93"/>
+      <c r="C26" s="92"/>
       <c r="D26" s="10"/>
       <c r="F26" s="36"/>
       <c r="G26" s="37"/>
@@ -4028,155 +4064,155 @@
       <c r="A38" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="129">
+      <c r="B38" s="128">
         <v>3</v>
       </c>
       <c r="C38" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="D38" s="143">
+      <c r="D38" s="142">
         <f>$D$19+7</f>
         <v>45978</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="121" t="s">
+      <c r="A39" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="B39" s="130" t="s">
+      <c r="B39" s="129" t="s">
         <v>15</v>
       </c>
-      <c r="C39" s="135" t="s">
+      <c r="C39" s="134" t="s">
         <v>7</v>
       </c>
-      <c r="D39" s="115" t="s">
+      <c r="D39" s="114" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="54" x14ac:dyDescent="0.25">
-      <c r="A40" s="122" t="s">
+      <c r="A40" s="121" t="s">
+        <v>30</v>
+      </c>
+      <c r="B40" s="111">
+        <v>2</v>
+      </c>
+      <c r="C40" s="133" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" s="117"/>
+    </row>
+    <row r="41" spans="1:8" ht="27" x14ac:dyDescent="0.25">
+      <c r="A41" s="119" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="112">
-        <v>2</v>
-      </c>
-      <c r="C40" s="134" t="s">
-        <v>69</v>
-      </c>
-      <c r="D40" s="118"/>
-    </row>
-    <row r="41" spans="1:8" ht="27" x14ac:dyDescent="0.25">
-      <c r="A41" s="120" t="s">
+      <c r="B41" s="111">
+        <v>1</v>
+      </c>
+      <c r="C41" s="135" t="s">
+        <v>50</v>
+      </c>
+      <c r="D41" s="118"/>
+    </row>
+    <row r="42" spans="1:8" ht="162" x14ac:dyDescent="0.25">
+      <c r="A42" s="132" t="s">
         <v>32</v>
       </c>
-      <c r="B41" s="112">
+      <c r="B42" s="111">
+        <v>5</v>
+      </c>
+      <c r="C42" s="112" t="s">
+        <v>60</v>
+      </c>
+      <c r="D42" s="112" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="54" x14ac:dyDescent="0.25">
+      <c r="A43" s="110" t="s">
+        <v>33</v>
+      </c>
+      <c r="B43" s="111">
         <v>1</v>
       </c>
-      <c r="C41" s="136" t="s">
-        <v>51</v>
-      </c>
-      <c r="D41" s="119"/>
-    </row>
-    <row r="42" spans="1:8" ht="162" x14ac:dyDescent="0.25">
-      <c r="A42" s="133" t="s">
-        <v>33</v>
-      </c>
-      <c r="B42" s="112">
-        <v>5</v>
-      </c>
-      <c r="C42" s="113" t="s">
+      <c r="C43" s="144" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43" s="112"/>
+    </row>
+    <row r="44" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="122"/>
+      <c r="B44" s="116"/>
+      <c r="C44" s="136" t="s">
         <v>61</v>
       </c>
-      <c r="D42" s="113" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="54" x14ac:dyDescent="0.25">
-      <c r="A43" s="111" t="s">
-        <v>34</v>
-      </c>
-      <c r="B43" s="112">
-        <v>1</v>
-      </c>
-      <c r="C43" s="145" t="s">
-        <v>35</v>
-      </c>
-      <c r="D43" s="113"/>
-    </row>
-    <row r="44" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="123"/>
-      <c r="B44" s="117"/>
-      <c r="C44" s="137" t="s">
-        <v>62</v>
-      </c>
-      <c r="D44" s="119"/>
+      <c r="D44" s="118"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="124" t="s">
+      <c r="A45" s="123" t="s">
         <v>21</v>
       </c>
-      <c r="B45" s="131">
+      <c r="B45" s="130">
         <v>9</v>
       </c>
-      <c r="C45" s="138" t="s">
-        <v>60</v>
+      <c r="C45" s="137" t="s">
+        <v>59</v>
       </c>
       <c r="D45" s="10"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="124"/>
-      <c r="B46" s="131"/>
-      <c r="C46" s="139"/>
+      <c r="A46" s="123"/>
+      <c r="B46" s="130"/>
+      <c r="C46" s="138"/>
       <c r="D46" s="10"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="125"/>
-      <c r="B47" s="131"/>
-      <c r="C47" s="139"/>
+      <c r="A47" s="124"/>
+      <c r="B47" s="130"/>
+      <c r="C47" s="138"/>
       <c r="D47" s="10"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="125"/>
-      <c r="B48" s="131"/>
-      <c r="C48" s="139"/>
+      <c r="A48" s="124"/>
+      <c r="B48" s="130"/>
+      <c r="C48" s="138"/>
       <c r="D48" s="10"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="125"/>
-      <c r="B49" s="131"/>
-      <c r="C49" s="139"/>
+      <c r="A49" s="124"/>
+      <c r="B49" s="130"/>
+      <c r="C49" s="138"/>
       <c r="D49" s="10"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="126"/>
-      <c r="B50" s="131"/>
-      <c r="C50" s="140"/>
+      <c r="A50" s="125"/>
+      <c r="B50" s="130"/>
+      <c r="C50" s="139"/>
       <c r="D50" s="51"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="126"/>
-      <c r="B51" s="131"/>
-      <c r="C51" s="140"/>
+      <c r="A51" s="125"/>
+      <c r="B51" s="130"/>
+      <c r="C51" s="139"/>
       <c r="D51" s="51"/>
     </row>
     <row r="52" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="127"/>
-      <c r="B52" s="131"/>
-      <c r="C52" s="141"/>
+      <c r="A52" s="126"/>
+      <c r="B52" s="130"/>
+      <c r="C52" s="140"/>
       <c r="D52" s="11"/>
     </row>
     <row r="53" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="128" t="s">
+      <c r="A53" s="127" t="s">
         <v>22</v>
       </c>
-      <c r="B53" s="132">
+      <c r="B53" s="131">
         <f>SUM(B40:B52)</f>
         <v>18</v>
       </c>
-      <c r="C53" s="142" t="s">
-        <v>63</v>
-      </c>
-      <c r="D53" s="144"/>
+      <c r="C53" s="141" t="s">
+        <v>62</v>
+      </c>
+      <c r="D53" s="143"/>
     </row>
     <row r="54" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="49"/>
@@ -4215,83 +4251,83 @@
     </row>
     <row r="57" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="5"/>
-      <c r="B57" s="95"/>
-      <c r="C57" s="103" t="s">
-        <v>45</v>
-      </c>
-      <c r="D57" s="94"/>
+      <c r="B57" s="94"/>
+      <c r="C57" s="102" t="s">
+        <v>44</v>
+      </c>
+      <c r="D57" s="93"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B58" s="4">
         <v>1</v>
       </c>
       <c r="C58" s="88" t="s">
+        <v>37</v>
+      </c>
+      <c r="D58" s="9" t="s">
         <v>38</v>
-      </c>
-      <c r="D58" s="9" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="54" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B59" s="2">
         <v>1</v>
       </c>
       <c r="C59" s="89" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D59" s="10"/>
     </row>
     <row r="60" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B60" s="2">
         <v>2</v>
       </c>
       <c r="C60" s="89" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D60" s="10"/>
     </row>
     <row r="61" spans="1:4" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B61" s="2">
         <v>1</v>
       </c>
       <c r="C61" s="89" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D61" s="10"/>
     </row>
     <row r="62" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B62" s="2">
         <v>2</v>
       </c>
       <c r="C62" s="89" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D62" s="10"/>
     </row>
     <row r="63" spans="1:4" ht="27" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B63" s="2">
         <v>2</v>
       </c>
       <c r="C63" s="89" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D63" s="10"/>
     </row>
@@ -4387,83 +4423,83 @@
     </row>
     <row r="75" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="5"/>
-      <c r="B75" s="95"/>
-      <c r="C75" s="103" t="s">
-        <v>67</v>
-      </c>
-      <c r="D75" s="94"/>
+      <c r="B75" s="94"/>
+      <c r="C75" s="102" t="s">
+        <v>66</v>
+      </c>
+      <c r="D75" s="93"/>
     </row>
     <row r="76" spans="1:4" ht="27" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B76" s="4">
         <v>2</v>
       </c>
-      <c r="C76" s="99" t="s">
-        <v>49</v>
+      <c r="C76" s="98" t="s">
+        <v>48</v>
       </c>
       <c r="D76" s="10"/>
     </row>
     <row r="77" spans="1:4" ht="27" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B77" s="2">
         <v>1</v>
       </c>
       <c r="C77" s="89" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D77" s="10"/>
     </row>
     <row r="78" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B78" s="2">
         <v>1</v>
       </c>
       <c r="C78" s="89" t="s">
-        <v>56</v>
-      </c>
-      <c r="D78" s="93" t="s">
-        <v>77</v>
+        <v>55</v>
+      </c>
+      <c r="D78" s="92" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="54" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B79" s="2">
         <v>2</v>
       </c>
       <c r="C79" s="89" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D79" s="10"/>
     </row>
     <row r="80" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B80" s="2">
         <v>2</v>
       </c>
       <c r="C80" s="89" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D80" s="10"/>
     </row>
     <row r="81" spans="1:4" ht="27" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B81" s="2">
         <v>1</v>
       </c>
       <c r="C81" s="89" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D81" s="10"/>
     </row>
@@ -4564,53 +4600,51 @@
       </c>
     </row>
     <row r="94" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="101"/>
-      <c r="B94" s="102"/>
-      <c r="C94" s="103" t="s">
-        <v>66</v>
-      </c>
-      <c r="D94" s="103"/>
-    </row>
-    <row r="95" spans="1:4" ht="27" x14ac:dyDescent="0.25">
-      <c r="A95" s="97" t="s">
+      <c r="A94" s="100"/>
+      <c r="B94" s="101"/>
+      <c r="C94" s="102" t="s">
+        <v>65</v>
+      </c>
+      <c r="D94" s="102"/>
+    </row>
+    <row r="95" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A95" s="96" t="s">
+        <v>77</v>
+      </c>
+      <c r="B95" s="97">
+        <v>3</v>
+      </c>
+      <c r="C95" s="89" t="s">
         <v>68</v>
       </c>
-      <c r="B95" s="98">
-        <v>3</v>
-      </c>
-      <c r="C95" s="89" t="s">
-        <v>70</v>
-      </c>
-      <c r="D95" s="104"/>
+      <c r="D95" s="103"/>
     </row>
     <row r="96" spans="1:4" ht="27" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B96" s="2">
         <v>3</v>
       </c>
       <c r="C96" s="89" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D96" s="10"/>
     </row>
     <row r="97" spans="1:4" ht="27" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B97" s="2">
         <v>3</v>
       </c>
-      <c r="C97" s="93" t="s">
-        <v>76</v>
+      <c r="C97" s="92" t="s">
+        <v>74</v>
       </c>
       <c r="D97" s="10"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
-        <v>72</v>
-      </c>
+      <c r="A98" s="1"/>
       <c r="B98" s="2"/>
       <c r="C98" s="10"/>
       <c r="D98" s="10"/>
@@ -4711,34 +4745,60 @@
         <v>13</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="5"/>
       <c r="B111" s="4"/>
-      <c r="C111" s="88"/>
+      <c r="C111" s="102" t="s">
+        <v>76</v>
+      </c>
       <c r="D111" s="9"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="1"/>
-      <c r="B112" s="2"/>
-      <c r="C112" s="90"/>
+    <row r="112" spans="1:4" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B112" s="2">
+        <v>4</v>
+      </c>
+      <c r="C112" s="92" t="s">
+        <v>82</v>
+      </c>
       <c r="D112" s="10"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="1"/>
-      <c r="B113" s="2"/>
-      <c r="C113" s="89"/>
-      <c r="D113" s="91"/>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="1"/>
-      <c r="B114" s="2"/>
-      <c r="C114" s="10"/>
+    <row r="113" spans="1:4" ht="81" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B113" s="2">
+        <v>2</v>
+      </c>
+      <c r="C113" s="89" t="s">
+        <v>83</v>
+      </c>
+      <c r="D113" s="90"/>
+    </row>
+    <row r="114" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B114" s="2">
+        <v>2</v>
+      </c>
+      <c r="C114" s="92" t="s">
+        <v>84</v>
+      </c>
       <c r="D114" s="10"/>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="1"/>
-      <c r="B115" s="2"/>
-      <c r="C115" s="10"/>
+    <row r="115" spans="1:4" ht="81" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B115" s="2">
+        <v>1</v>
+      </c>
+      <c r="C115" s="92" t="s">
+        <v>85</v>
+      </c>
       <c r="D115" s="10"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -4807,10 +4867,10 @@
       </c>
       <c r="B126" s="47">
         <f>SUM(B111:B125)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C126" s="87" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D126" s="48"/>
     </row>
@@ -4852,13 +4912,13 @@
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="5"/>
       <c r="B130" s="4"/>
-      <c r="C130" s="92"/>
+      <c r="C130" s="91"/>
       <c r="D130" s="9"/>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="2"/>
-      <c r="C131" s="93"/>
+      <c r="C131" s="92"/>
       <c r="D131" s="10"/>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -5024,17 +5084,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Belge" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="14" ma:contentTypeDescription="Yeni belge oluşturun." ma:contentTypeScope="" ma:versionID="ee0afad02cec1cb5c008e069b7696935">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="071b3019c14a3acff1c11c5229ff0248" ns2:_="" ns3:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -5263,6 +5312,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
   <ds:schemaRefs>
@@ -5272,17 +5332,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15235525-7A96-4FDC-BE0C-FC0EC8076A2A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5299,4 +5348,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
doc(): mise à jour et ajout de documentation
</commit_message>
<xml_diff>
--- a/T-P_App-MatiasDenis-JDT.xlsx
+++ b/T-P_App-MatiasDenis-JDT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\05-repertoires-ict-ssd (2022)\Deuxième année\P_App\P_App-Bruteforce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8210AA-E95C-4300-A7E7-85E6C33982D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D02A79-B5E9-401E-8AC1-11D43BE97C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees" sheetId="7" r:id="rId1"/>
@@ -36,6 +36,7 @@
   <customWorkbookViews>
     <customWorkbookView name="Gilbert Gruaz - Affichage personnalisé" guid="{4120A410-7ADA-42AD-8010-013327A2ECF1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="821" activeSheetId="4"/>
   </customWorkbookViews>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="89">
   <si>
     <t>Module :</t>
   </si>
@@ -249,9 +250,6 @@
     <t>Modification du script principal pour utiliser le test FTP réel, tests de bruteforce avec wordlist simple, validation de la détection correcte du mot de passe via FTP, mesure du temps et du nombre de tentatives. Tâche terminée.</t>
   </si>
   <si>
-    <t>Tests du programme avec des positions différentes du mot de passe dans la wordlist et calcul du temps. D'autres tests à faire afin d'optimiser le programme. Tâche en cours.</t>
-  </si>
-  <si>
     <t>Maladie.</t>
   </si>
   <si>
@@ -280,9 +278,6 @@
   </si>
   <si>
     <t>Il y avait confusion dans les dates où le projet a été effectué mais tout est juste maintenant. Tâche terminée.</t>
-  </si>
-  <si>
-    <t>Changement dans le rapport de travail: réduction du nombre de page pour s'aligner avec ce qui est demandé dans le cahier des charges. Tâche en cours.</t>
   </si>
   <si>
     <t>Tests</t>
@@ -339,6 +334,21 @@
     <t>Chaque service a été testé individuellement afin de vérifier son bon fonctionnement et son accessibilité locale.
 Le bruteforce FTP a été validé par la découverte du mot de passe, tandis que les services HTTP et SSH ont été vérifiés par des tests d’authentification et l’analyse des logs.
 Ces tests ont permis de confirmer que l’ensemble du projet fonctionne correctement et conformément aux objectifs définis.</t>
+  </si>
+  <si>
+    <t>Tests du programme avec des positions différentes du mot de passe dans la wordlist et calcul du temps. D'autres tests à faire afin d'optimiser le programme. Tâche terminée.</t>
+  </si>
+  <si>
+    <t>Changement dans le rapport de travail: réduction du nombre de page pour s'aligner avec ce qui est demandé dans le cahier des charges. Tâche terminée.</t>
+  </si>
+  <si>
+    <t>Enregistrement de la vidéo pour le rendu du projet</t>
+  </si>
+  <si>
+    <t>A l'aide de powerpoint, une vidéo de démonstration du programme a été enregistrée afin de démontrer ce qu'il fait.</t>
+  </si>
+  <si>
+    <t>Rendu final du projet</t>
   </si>
 </sst>
 </file>
@@ -1198,7 +1208,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="149">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1456,10 +1466,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -1653,6 +1659,14 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -2303,7 +2317,7 @@
   <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" topLeftCell="A22" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2519,10 +2533,10 @@
     </row>
     <row r="19" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="78"/>
-      <c r="B19" s="145" t="s">
+      <c r="B19" s="144" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="146"/>
+      <c r="C19" s="145"/>
       <c r="D19" s="59"/>
       <c r="E19" s="59"/>
       <c r="F19" s="59"/>
@@ -2729,7 +2743,7 @@
         <v>15</v>
       </c>
       <c r="C35" s="70" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D35" s="59"/>
       <c r="E35" s="59"/>
@@ -2742,7 +2756,7 @@
         <v>16</v>
       </c>
       <c r="C36" s="70" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D36" s="59"/>
       <c r="E36" s="59"/>
@@ -2755,7 +2769,7 @@
         <v>17</v>
       </c>
       <c r="C37" s="70" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D37" s="59"/>
       <c r="E37" s="59"/>
@@ -2768,7 +2782,7 @@
         <v>18</v>
       </c>
       <c r="C38" s="71" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D38" s="59"/>
       <c r="E38" s="59"/>
@@ -2781,7 +2795,7 @@
         <v>19</v>
       </c>
       <c r="C39" s="70" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D39" s="59"/>
       <c r="E39" s="59"/>
@@ -2794,7 +2808,7 @@
         <v>20</v>
       </c>
       <c r="C40" s="71" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D40" s="59"/>
       <c r="E40" s="59"/>
@@ -2806,7 +2820,9 @@
       <c r="B41" s="81">
         <v>21</v>
       </c>
-      <c r="C41" s="71"/>
+      <c r="C41" s="71" t="s">
+        <v>86</v>
+      </c>
       <c r="D41" s="59"/>
       <c r="E41" s="59"/>
       <c r="F41" s="59"/>
@@ -2955,27 +2971,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -3005,27 +3021,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -3064,7 +3080,7 @@
     </row>
     <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
-      <c r="B3" s="147" t="s">
+      <c r="B3" s="146" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="16">
@@ -3073,7 +3089,7 @@
     </row>
     <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
-      <c r="B4" s="148"/>
+      <c r="B4" s="147"/>
       <c r="C4" s="22">
         <v>0</v>
       </c>
@@ -3734,8 +3750,8 @@
   <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:H147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="C117" sqref="C117"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="C135" sqref="C135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -3763,38 +3779,38 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="114" t="s">
+      <c r="A2" s="113" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="114" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="114" t="s">
+      <c r="C2" s="113" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="114" t="s">
+      <c r="D2" s="113" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="100"/>
-      <c r="B3" s="101"/>
-      <c r="C3" s="102" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" s="102"/>
+      <c r="A3" s="99"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="101" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="101"/>
     </row>
     <row r="4" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="96" t="s">
+      <c r="A4" s="95" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="97">
+      <c r="B4" s="96">
         <v>9</v>
       </c>
-      <c r="C4" s="98" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="99"/>
+      <c r="C4" s="97" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="98"/>
     </row>
     <row r="5" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -3917,35 +3933,35 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="95"/>
-      <c r="B21" s="94"/>
-      <c r="C21" s="93" t="s">
-        <v>64</v>
-      </c>
-      <c r="D21" s="93"/>
+      <c r="A21" s="94"/>
+      <c r="B21" s="93"/>
+      <c r="C21" s="92" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="92"/>
     </row>
     <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="110"/>
-      <c r="B22" s="111"/>
-      <c r="C22" s="112"/>
-      <c r="D22" s="113"/>
+      <c r="A22" s="109"/>
+      <c r="B22" s="110"/>
+      <c r="C22" s="111"/>
+      <c r="D22" s="112"/>
     </row>
     <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="106"/>
-      <c r="B23" s="107"/>
-      <c r="C23" s="108"/>
-      <c r="D23" s="109"/>
+      <c r="A23" s="105"/>
+      <c r="B23" s="106"/>
+      <c r="C23" s="107"/>
+      <c r="D23" s="108"/>
     </row>
     <row r="24" spans="1:8" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A24" s="96"/>
-      <c r="B24" s="104"/>
-      <c r="C24" s="105"/>
-      <c r="D24" s="105"/>
+      <c r="A24" s="95"/>
+      <c r="B24" s="103"/>
+      <c r="C24" s="104"/>
+      <c r="D24" s="104"/>
     </row>
     <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
-      <c r="C25" s="92"/>
+      <c r="C25" s="91"/>
       <c r="D25" s="10"/>
       <c r="F25" s="34"/>
       <c r="G25" s="30"/>
@@ -3954,7 +3970,7 @@
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
-      <c r="C26" s="92"/>
+      <c r="C26" s="91"/>
       <c r="D26" s="10"/>
       <c r="F26" s="36"/>
       <c r="G26" s="37"/>
@@ -4064,155 +4080,155 @@
       <c r="A38" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="128">
+      <c r="B38" s="127">
         <v>3</v>
       </c>
       <c r="C38" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="D38" s="142">
+      <c r="D38" s="141">
         <f>$D$19+7</f>
         <v>45978</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="120" t="s">
+      <c r="A39" s="119" t="s">
         <v>3</v>
       </c>
-      <c r="B39" s="129" t="s">
+      <c r="B39" s="128" t="s">
         <v>15</v>
       </c>
-      <c r="C39" s="134" t="s">
+      <c r="C39" s="133" t="s">
         <v>7</v>
       </c>
-      <c r="D39" s="114" t="s">
+      <c r="D39" s="113" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="54" x14ac:dyDescent="0.25">
-      <c r="A40" s="121" t="s">
+      <c r="A40" s="120" t="s">
         <v>30</v>
       </c>
-      <c r="B40" s="111">
+      <c r="B40" s="110">
         <v>2</v>
       </c>
-      <c r="C40" s="133" t="s">
-        <v>67</v>
-      </c>
-      <c r="D40" s="117"/>
+      <c r="C40" s="132" t="s">
+        <v>66</v>
+      </c>
+      <c r="D40" s="116"/>
     </row>
     <row r="41" spans="1:8" ht="27" x14ac:dyDescent="0.25">
-      <c r="A41" s="119" t="s">
+      <c r="A41" s="118" t="s">
         <v>31</v>
       </c>
-      <c r="B41" s="111">
+      <c r="B41" s="110">
         <v>1</v>
       </c>
-      <c r="C41" s="135" t="s">
+      <c r="C41" s="134" t="s">
         <v>50</v>
       </c>
-      <c r="D41" s="118"/>
+      <c r="D41" s="117"/>
     </row>
     <row r="42" spans="1:8" ht="162" x14ac:dyDescent="0.25">
-      <c r="A42" s="132" t="s">
+      <c r="A42" s="131" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="111">
+      <c r="B42" s="110">
         <v>5</v>
       </c>
-      <c r="C42" s="112" t="s">
+      <c r="C42" s="111" t="s">
+        <v>59</v>
+      </c>
+      <c r="D42" s="111" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="54" x14ac:dyDescent="0.25">
+      <c r="A43" s="109" t="s">
+        <v>33</v>
+      </c>
+      <c r="B43" s="110">
+        <v>1</v>
+      </c>
+      <c r="C43" s="143" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43" s="111"/>
+    </row>
+    <row r="44" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="121"/>
+      <c r="B44" s="115"/>
+      <c r="C44" s="135" t="s">
         <v>60</v>
       </c>
-      <c r="D42" s="112" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="54" x14ac:dyDescent="0.25">
-      <c r="A43" s="110" t="s">
-        <v>33</v>
-      </c>
-      <c r="B43" s="111">
-        <v>1</v>
-      </c>
-      <c r="C43" s="144" t="s">
-        <v>34</v>
-      </c>
-      <c r="D43" s="112"/>
-    </row>
-    <row r="44" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="122"/>
-      <c r="B44" s="116"/>
-      <c r="C44" s="136" t="s">
-        <v>61</v>
-      </c>
-      <c r="D44" s="118"/>
+      <c r="D44" s="117"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="123" t="s">
+      <c r="A45" s="122" t="s">
         <v>21</v>
       </c>
-      <c r="B45" s="130">
+      <c r="B45" s="129">
         <v>9</v>
       </c>
-      <c r="C45" s="137" t="s">
-        <v>59</v>
+      <c r="C45" s="136" t="s">
+        <v>58</v>
       </c>
       <c r="D45" s="10"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="123"/>
-      <c r="B46" s="130"/>
-      <c r="C46" s="138"/>
+      <c r="A46" s="122"/>
+      <c r="B46" s="129"/>
+      <c r="C46" s="137"/>
       <c r="D46" s="10"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="124"/>
-      <c r="B47" s="130"/>
-      <c r="C47" s="138"/>
+      <c r="A47" s="123"/>
+      <c r="B47" s="129"/>
+      <c r="C47" s="137"/>
       <c r="D47" s="10"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="124"/>
-      <c r="B48" s="130"/>
-      <c r="C48" s="138"/>
+      <c r="A48" s="123"/>
+      <c r="B48" s="129"/>
+      <c r="C48" s="137"/>
       <c r="D48" s="10"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="124"/>
-      <c r="B49" s="130"/>
-      <c r="C49" s="138"/>
+      <c r="A49" s="123"/>
+      <c r="B49" s="129"/>
+      <c r="C49" s="137"/>
       <c r="D49" s="10"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="125"/>
-      <c r="B50" s="130"/>
-      <c r="C50" s="139"/>
+      <c r="A50" s="124"/>
+      <c r="B50" s="129"/>
+      <c r="C50" s="138"/>
       <c r="D50" s="51"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="125"/>
-      <c r="B51" s="130"/>
-      <c r="C51" s="139"/>
+      <c r="A51" s="124"/>
+      <c r="B51" s="129"/>
+      <c r="C51" s="138"/>
       <c r="D51" s="51"/>
     </row>
     <row r="52" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="126"/>
-      <c r="B52" s="130"/>
-      <c r="C52" s="140"/>
+      <c r="A52" s="125"/>
+      <c r="B52" s="129"/>
+      <c r="C52" s="139"/>
       <c r="D52" s="11"/>
     </row>
     <row r="53" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="127" t="s">
+      <c r="A53" s="126" t="s">
         <v>22</v>
       </c>
-      <c r="B53" s="131">
+      <c r="B53" s="130">
         <f>SUM(B40:B52)</f>
         <v>18</v>
       </c>
-      <c r="C53" s="141" t="s">
-        <v>62</v>
-      </c>
-      <c r="D53" s="143"/>
+      <c r="C53" s="140" t="s">
+        <v>61</v>
+      </c>
+      <c r="D53" s="142"/>
     </row>
     <row r="54" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="49"/>
@@ -4251,11 +4267,11 @@
     </row>
     <row r="57" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="5"/>
-      <c r="B57" s="94"/>
-      <c r="C57" s="102" t="s">
+      <c r="B57" s="93"/>
+      <c r="C57" s="101" t="s">
         <v>44</v>
       </c>
-      <c r="D57" s="93"/>
+      <c r="D57" s="92"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
@@ -4291,7 +4307,7 @@
         <v>2</v>
       </c>
       <c r="C60" s="89" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D60" s="10"/>
     </row>
@@ -4315,7 +4331,7 @@
         <v>2</v>
       </c>
       <c r="C62" s="89" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D62" s="10"/>
     </row>
@@ -4327,7 +4343,7 @@
         <v>2</v>
       </c>
       <c r="C63" s="89" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D63" s="10"/>
     </row>
@@ -4423,11 +4439,11 @@
     </row>
     <row r="75" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="5"/>
-      <c r="B75" s="94"/>
-      <c r="C75" s="102" t="s">
-        <v>66</v>
-      </c>
-      <c r="D75" s="93"/>
+      <c r="B75" s="93"/>
+      <c r="C75" s="101" t="s">
+        <v>65</v>
+      </c>
+      <c r="D75" s="92"/>
     </row>
     <row r="76" spans="1:4" ht="27" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
@@ -4436,7 +4452,7 @@
       <c r="B76" s="4">
         <v>2</v>
       </c>
-      <c r="C76" s="98" t="s">
+      <c r="C76" s="97" t="s">
         <v>48</v>
       </c>
       <c r="D76" s="10"/>
@@ -4463,8 +4479,8 @@
       <c r="C78" s="89" t="s">
         <v>55</v>
       </c>
-      <c r="D78" s="92" t="s">
-        <v>75</v>
+      <c r="D78" s="91" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="54" x14ac:dyDescent="0.25">
@@ -4499,7 +4515,7 @@
         <v>1</v>
       </c>
       <c r="C81" s="89" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="D81" s="10"/>
     </row>
@@ -4600,24 +4616,24 @@
       </c>
     </row>
     <row r="94" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="100"/>
-      <c r="B94" s="101"/>
-      <c r="C94" s="102" t="s">
-        <v>65</v>
-      </c>
-      <c r="D94" s="102"/>
+      <c r="A94" s="99"/>
+      <c r="B94" s="100"/>
+      <c r="C94" s="101" t="s">
+        <v>64</v>
+      </c>
+      <c r="D94" s="101"/>
     </row>
     <row r="95" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A95" s="96" t="s">
-        <v>77</v>
-      </c>
-      <c r="B95" s="97">
+      <c r="A95" s="95" t="s">
+        <v>75</v>
+      </c>
+      <c r="B95" s="96">
         <v>3</v>
       </c>
       <c r="C95" s="89" t="s">
-        <v>68</v>
-      </c>
-      <c r="D95" s="103"/>
+        <v>67</v>
+      </c>
+      <c r="D95" s="102"/>
     </row>
     <row r="96" spans="1:4" ht="27" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
@@ -4627,7 +4643,7 @@
         <v>3</v>
       </c>
       <c r="C96" s="89" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="D96" s="10"/>
     </row>
@@ -4638,8 +4654,8 @@
       <c r="B97" s="2">
         <v>3</v>
       </c>
-      <c r="C97" s="92" t="s">
-        <v>74</v>
+      <c r="C97" s="91" t="s">
+        <v>72</v>
       </c>
       <c r="D97" s="10"/>
     </row>
@@ -4748,56 +4764,56 @@
     <row r="111" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="5"/>
       <c r="B111" s="4"/>
-      <c r="C111" s="102" t="s">
-        <v>76</v>
+      <c r="C111" s="101" t="s">
+        <v>74</v>
       </c>
       <c r="D111" s="9"/>
     </row>
     <row r="112" spans="1:4" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B112" s="2">
         <v>4</v>
       </c>
-      <c r="C112" s="92" t="s">
-        <v>82</v>
+      <c r="C112" s="91" t="s">
+        <v>80</v>
       </c>
       <c r="D112" s="10"/>
     </row>
     <row r="113" spans="1:4" ht="81" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B113" s="2">
         <v>2</v>
       </c>
       <c r="C113" s="89" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D113" s="90"/>
     </row>
     <row r="114" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B114" s="2">
         <v>2</v>
       </c>
-      <c r="C114" s="92" t="s">
-        <v>84</v>
+      <c r="C114" s="91" t="s">
+        <v>82</v>
       </c>
       <c r="D114" s="10"/>
     </row>
     <row r="115" spans="1:4" ht="81" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B115" s="2">
         <v>1</v>
       </c>
-      <c r="C115" s="92" t="s">
-        <v>85</v>
+      <c r="C115" s="91" t="s">
+        <v>83</v>
       </c>
       <c r="D115" s="10"/>
     </row>
@@ -4909,16 +4925,24 @@
         <v>13</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="5"/>
-      <c r="B130" s="4"/>
-      <c r="C130" s="91"/>
+    <row r="130" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A130" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B130" s="4">
+        <v>2</v>
+      </c>
+      <c r="C130" s="148" t="s">
+        <v>87</v>
+      </c>
       <c r="D130" s="9"/>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="2"/>
-      <c r="C131" s="92"/>
+      <c r="C131" s="149" t="s">
+        <v>88</v>
+      </c>
       <c r="D131" s="10"/>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -5005,7 +5029,7 @@
       </c>
       <c r="B145" s="47">
         <f>SUM(B130:B144)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C145" s="87" t="s">
         <v>28</v>
@@ -5084,6 +5108,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Belge" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="14" ma:contentTypeDescription="Yeni belge oluşturun." ma:contentTypeScope="" ma:versionID="ee0afad02cec1cb5c008e069b7696935">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="071b3019c14a3acff1c11c5229ff0248" ns2:_="" ns3:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -5312,17 +5347,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
   <ds:schemaRefs>
@@ -5332,6 +5356,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15235525-7A96-4FDC-BE0C-FC0EC8076A2A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5348,15 +5383,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>